<commit_message>
Cambios de la reunion sobre el anémico de contextos
</commit_message>
<xml_diff>
--- a/Doo-Doc/Nueva Version Victus/MuestreoDatos/Agenda Muestreo Datos.xlsx
+++ b/Doo-Doc/Nueva Version Victus/MuestreoDatos/Agenda Muestreo Datos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Music\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uconet-my.sharepoint.com/personal/juan_avendano1956_uco_net_co/Documents/Documents/victus-doc/Doo-Doc/Nueva Version Victus/MuestreoDatos/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEA397AB-45D2-4B42-8BF3-D633A0A4C278}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2D4B8DA6-DD27-486A-88C5-FC69C929F1D2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{2D4B8DA6-DD27-486A-88C5-FC69C929F1D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Objetos de dominio" sheetId="1" r:id="rId1"/>
@@ -436,7 +436,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -506,7 +506,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -824,11 +824,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ADC7617-6509-431F-A99E-8882BF74D5E4}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="27.6640625" customWidth="1"/>
     <col min="2" max="2" width="58.33203125" customWidth="1"/>
@@ -884,7 +884,7 @@
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="21.6640625" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
@@ -1071,7 +1071,7 @@
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="40.44140625" customWidth="1"/>
     <col min="3" max="3" width="40.5546875" customWidth="1"/>
@@ -1292,11 +1292,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1481DBD8-8614-460B-A4B3-0BC96282F835}">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.109375" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>

</xml_diff>

<commit_message>
Nivel superado con el modelo de dominio y muestreo de datos
</commit_message>
<xml_diff>
--- a/Doo-Doc/Nueva Version Victus/MuestreoDatos/Agenda Muestreo Datos.xlsx
+++ b/Doo-Doc/Nueva Version Victus/MuestreoDatos/Agenda Muestreo Datos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Music\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEA397AB-45D2-4B42-8BF3-D633A0A4C278}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B89AD7CE-8143-4AEB-B50A-6CDFA11B9B51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2D4B8DA6-DD27-486A-88C5-FC69C929F1D2}"/>
+    <workbookView xWindow="15855" yWindow="1725" windowWidth="20220" windowHeight="15345" activeTab="2" xr2:uid="{2D4B8DA6-DD27-486A-88C5-FC69C929F1D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Objetos de dominio" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="67">
   <si>
     <t>Nombre</t>
   </si>
@@ -200,9 +200,6 @@
     <t>Capacidad</t>
   </si>
   <si>
-    <t>tiempoUsoDia</t>
-  </si>
-  <si>
     <t>Normas</t>
   </si>
   <si>
@@ -215,9 +212,6 @@
     <t>Es un espacio deportivo y lúdico</t>
   </si>
   <si>
-    <t>1 hora</t>
-  </si>
-  <si>
     <t>Para reservar la psicina debe contar con 1 dia de anterioridad</t>
   </si>
   <si>
@@ -227,9 +221,6 @@
     <t>Espacio que cuenta con diferentes maquinas para la ejercitación</t>
   </si>
   <si>
-    <t>2 horas</t>
-  </si>
-  <si>
     <t>Usar la maquinaria con toalla y mantener la higiene</t>
   </si>
   <si>
@@ -240,6 +231,18 @@
   </si>
   <si>
     <t>Corresponde a los turnos que un residente puede reservar en una agenda, es decir, el residente toma un turno que esta disponible de una agenda que anteriormente ya esta programada.</t>
+  </si>
+  <si>
+    <t>tiempoUso</t>
+  </si>
+  <si>
+    <t>unidadDeTiempoUso</t>
+  </si>
+  <si>
+    <t>Minutos</t>
+  </si>
+  <si>
+    <t>Hora</t>
   </si>
 </sst>
 </file>
@@ -250,7 +253,7 @@
     <numFmt numFmtId="164" formatCode="dddd\,\ d\ &quot;de&quot;\ mmmm\ &quot;de&quot;\ yyyy\ h:mm:ss\ AM/PM"/>
     <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -284,6 +287,28 @@
     <font>
       <sz val="8"/>
       <color rgb="FF4EA72E"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="16"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -367,7 +392,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -395,42 +420,60 @@
     <xf numFmtId="49" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -463,8 +506,8 @@
       <sheetName val="Administrador"/>
       <sheetName val="ConjuntoResidencial"/>
       <sheetName val="Zonainmueble"/>
+      <sheetName val="Inmueble"/>
       <sheetName val="ZonaComun"/>
-      <sheetName val="Inmueble"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
@@ -482,24 +525,24 @@
         </row>
       </sheetData>
       <sheetData sheetId="3"/>
-      <sheetData sheetId="4">
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5">
         <row r="4">
           <cell r="I4" t="str">
-            <v>Piscina-1-Forest apartamentos</v>
+            <v>1-Forest apartamentos</v>
           </cell>
         </row>
         <row r="5">
           <cell r="I5" t="str">
-            <v>Gimnasio-1-Forest apartamentos</v>
+            <v>1-Forest apartamentos</v>
           </cell>
         </row>
         <row r="6">
           <cell r="I6" t="str">
-            <v>piscinaAdultos-2-Natural</v>
+            <v>2-Natural</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="5"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -824,17 +867,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ADC7617-6509-431F-A99E-8882BF74D5E4}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.6640625" customWidth="1"/>
-    <col min="2" max="2" width="58.33203125" customWidth="1"/>
+    <col min="1" max="1" width="27.7109375" customWidth="1"/>
+    <col min="2" max="2" width="58.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -842,7 +885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -850,20 +893,20 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -878,37 +921,38 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AAB45A7-2401-4156-812B-1376902CA2CF}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E1"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="21.6640625" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
     <col min="4" max="4" width="27" customWidth="1"/>
-    <col min="5" max="6" width="21.6640625" customWidth="1"/>
-    <col min="7" max="7" width="15" customWidth="1"/>
-    <col min="8" max="8" width="23.6640625" customWidth="1"/>
-    <col min="9" max="9" width="33.109375" customWidth="1"/>
+    <col min="5" max="7" width="21.7109375" customWidth="1"/>
+    <col min="8" max="8" width="15" customWidth="1"/>
+    <col min="9" max="9" width="23.7109375" customWidth="1"/>
+    <col min="10" max="10" width="33.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="37" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="6"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="31"/>
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
       <c r="I1" s="6"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J1" s="6"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>42</v>
       </c>
@@ -925,17 +969,18 @@
         <v>46</v>
       </c>
       <c r="F2" s="7"/>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="7"/>
+      <c r="H2" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="I2" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="J2" s="7" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -952,102 +997,114 @@
         <v>51</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="I3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I3" s="32" t="s">
+    </row>
+    <row r="4" spans="1:10" ht="76.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="32">
+        <v>1</v>
+      </c>
+      <c r="B4" s="32" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="29">
-        <v>1</v>
-      </c>
-      <c r="B4" s="29" t="s">
+      <c r="C4" s="33"/>
+      <c r="D4" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="35">
+        <v>50</v>
+      </c>
+      <c r="F4" s="35">
+        <v>60</v>
+      </c>
+      <c r="G4" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="H4" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E4" s="33">
-        <v>50</v>
-      </c>
-      <c r="F4" s="29" t="s">
-        <v>57</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="H4" s="29" t="str">
+      <c r="I4" s="25" t="str">
         <f>[1]ConjuntoResidencial!$G$4</f>
         <v>1-Forest apartamentos</v>
       </c>
-      <c r="I4" s="34" t="str">
-        <f>_xlfn.CONCAT(B4,"-",H4)</f>
+      <c r="J4" s="29" t="str">
+        <f>_xlfn.CONCAT(B4,"-",I4)</f>
         <v>Piscina-1-Forest apartamentos</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="5">
+    <row r="5" spans="1:10" ht="84" x14ac:dyDescent="0.35">
+      <c r="A5" s="36">
         <v>2</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="36" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" s="36"/>
+      <c r="D5" s="37" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5" s="38">
+        <v>20</v>
+      </c>
+      <c r="F5" s="38">
+        <v>120</v>
+      </c>
+      <c r="G5" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="H5" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="35" t="s">
-        <v>60</v>
-      </c>
-      <c r="E5" s="36">
-        <v>20</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="G5" s="35" t="s">
-        <v>62</v>
-      </c>
-      <c r="H5" s="29" t="str">
+      <c r="I5" s="25" t="str">
         <f>[1]ConjuntoResidencial!$G$4</f>
         <v>1-Forest apartamentos</v>
       </c>
-      <c r="I5" s="34" t="str">
-        <f>_xlfn.CONCAT(B5,"-",H5)</f>
+      <c r="J5" s="29" t="str">
+        <f>_xlfn.CONCAT(B5,"-",I5)</f>
         <v>Gimnasio-1-Forest apartamentos</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="5">
+    <row r="6" spans="1:10" ht="76.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="36">
         <v>3</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="3" t="s">
+      <c r="B6" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="36"/>
+      <c r="D6" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="E6" s="38">
+        <v>15</v>
+      </c>
+      <c r="F6" s="38">
+        <v>1</v>
+      </c>
+      <c r="G6" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="H6" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E6" s="36">
-        <v>15</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="H6" s="29" t="str">
+      <c r="I6" s="25" t="str">
         <f>[1]ConjuntoResidencial!$G$5</f>
         <v>2-Natural</v>
       </c>
-      <c r="I6" s="34" t="str">
-        <f>_xlfn.CONCAT(B6,"-",H6)</f>
+      <c r="J6" s="29" t="str">
+        <f>_xlfn.CONCAT(B6,"-",I6)</f>
         <v>piscinaAdultos-2-Natural</v>
       </c>
     </row>
@@ -1057,7 +1114,7 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Objetos de dominio'!A1" display="&lt;&lt;&lt;&lt;&lt;&lt; Volver al inicio" xr:uid="{42E27472-290F-498E-8D59-E2019AE03564}"/>
-    <hyperlink ref="I1" location="Objetos de dominio!A1" display="Objetos de dominio!A1" xr:uid="{66BB4A93-8C9D-4AFA-80A4-F6947BF9E083}"/>
+    <hyperlink ref="J1" location="Objetos de dominio!A1" display="Objetos de dominio!A1" xr:uid="{66BB4A93-8C9D-4AFA-80A4-F6947BF9E083}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1067,31 +1124,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4578BD62-C112-42DC-9A20-08C85087F0AF}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E1"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="40.44140625" customWidth="1"/>
-    <col min="3" max="3" width="40.5546875" customWidth="1"/>
-    <col min="4" max="4" width="17.33203125" customWidth="1"/>
-    <col min="5" max="5" width="46.109375" customWidth="1"/>
-    <col min="6" max="6" width="44.77734375" customWidth="1"/>
-    <col min="7" max="7" width="128.44140625" customWidth="1"/>
+    <col min="2" max="2" width="40.42578125" customWidth="1"/>
+    <col min="3" max="3" width="40.5703125" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" customWidth="1"/>
+    <col min="5" max="5" width="46.140625" customWidth="1"/>
+    <col min="6" max="6" width="44.7109375" customWidth="1"/>
+    <col min="7" max="7" width="128.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="37" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>8</v>
       </c>
@@ -1108,11 +1165,11 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -1131,13 +1188,13 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>1</v>
       </c>
-      <c r="B4" s="10" t="str">
+      <c r="B4" s="40" t="str">
         <f>[1]ZonaComun!$I$5</f>
-        <v>Gimnasio-1-Forest apartamentos</v>
+        <v>1-Forest apartamentos</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>18</v>
@@ -1153,16 +1210,16 @@
       </c>
       <c r="G4" s="8" t="str">
         <f>C4&amp;" "&amp;TEXT(E4,"- dd  mmmm yyyy h:mm:ss AM/PM ")&amp;" hasta "&amp;TEXT(F4,"- dd  mmmm yyyy h:mm:ss AM/PM ")&amp;"-"&amp;B4</f>
-        <v>Agenda para residentes turno Diurno - 18  septiembre 2024 6:00:00 a. m.  hasta - 18  septiembre 2024 2:00:00 p. m. -Gimnasio-1-Forest apartamentos</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+        <v>Agenda para residentes turno Diurno - 18  septiembre 2024 6:00:00 a. m.  hasta - 18  septiembre 2024 2:00:00 p. m. -1-Forest apartamentos</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <v>2</v>
       </c>
-      <c r="B5" s="10" t="str">
+      <c r="B5" s="40" t="str">
         <f>[1]ZonaComun!$I$5</f>
-        <v>Gimnasio-1-Forest apartamentos</v>
+        <v>1-Forest apartamentos</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>20</v>
@@ -1178,16 +1235,16 @@
       </c>
       <c r="G5" s="8" t="str">
         <f t="shared" ref="G5:G7" si="0">C5&amp;" "&amp;TEXT(E5,"- dd  mmmm yyyy h:mm:ss AM/PM ")&amp;" hasta "&amp;TEXT(F5,"- dd  mmmm yyyy h:mm:ss AM/PM ")&amp;"-"&amp;B5</f>
-        <v>Agenda para residentes turno Nocturno - 18  septiembre 2024 3:00:00 p. m.  hasta - 18  septiembre 2024 9:00:00 p. m. -Gimnasio-1-Forest apartamentos</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+        <v>Agenda para residentes turno Nocturno - 18  septiembre 2024 3:00:00 p. m.  hasta - 18  septiembre 2024 9:00:00 p. m. -1-Forest apartamentos</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>3</v>
       </c>
-      <c r="B6" s="10" t="str">
+      <c r="B6" s="40" t="str">
         <f>[1]ZonaComun!$I$6</f>
-        <v>piscinaAdultos-2-Natural</v>
+        <v>2-Natural</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>21</v>
@@ -1203,16 +1260,16 @@
       </c>
       <c r="G6" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>Agenda para residentes - 20  septiembre 2024 10:00:00 a. m.  hasta - 20  septiembre 2024 1:00:00 p. m. -piscinaAdultos-2-Natural</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+        <v>Agenda para residentes - 20  septiembre 2024 10:00:00 a. m.  hasta - 20  septiembre 2024 1:00:00 p. m. -2-Natural</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
         <v>4</v>
       </c>
-      <c r="B7" s="10" t="str">
+      <c r="B7" s="40" t="str">
         <f>[1]ZonaComun!$I$4</f>
-        <v>Piscina-1-Forest apartamentos</v>
+        <v>1-Forest apartamentos</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>22</v>
@@ -1228,10 +1285,10 @@
       </c>
       <c r="G7" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>Agenda para dias de mantenimiento - 18  septiembre 2024 8:00:00 a. m.  hasta - 18  septiembre 2024 12:00:00 p. m. -Piscina-1-Forest apartamentos</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+        <v>Agenda para dias de mantenimiento - 18  septiembre 2024 8:00:00 a. m.  hasta - 18  septiembre 2024 12:00:00 p. m. -1-Forest apartamentos</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="10"/>
       <c r="C8" s="9"/>
@@ -1240,7 +1297,7 @@
       <c r="F8" s="11"/>
       <c r="G8" s="8"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="9"/>
       <c r="B9" s="10"/>
       <c r="C9" s="9"/>
@@ -1249,7 +1306,7 @@
       <c r="F9" s="11"/>
       <c r="G9" s="8"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="10"/>
       <c r="C10" s="5"/>
@@ -1258,7 +1315,7 @@
       <c r="F10" s="11"/>
       <c r="G10" s="8"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="9"/>
       <c r="B11" s="10"/>
       <c r="C11" s="5"/>
@@ -1267,12 +1324,12 @@
       <c r="F11" s="11"/>
       <c r="G11" s="8"/>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>24</v>
       </c>
@@ -1283,6 +1340,11 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Objetos de dominio'!A1" display="&lt;&lt;&lt;&lt;&lt;&lt; Volver al inicio" xr:uid="{80B0E295-9C45-4B66-99DF-E7CF9E9791FC}"/>
+    <hyperlink ref="B3" location="ZonaComun!A1" display="ZonaComun" xr:uid="{23A414B0-B4D1-4009-AD81-8FE561EAB17A}"/>
+    <hyperlink ref="B4" location="ZonaComun!A5" display="ZonaComun!A5" xr:uid="{0759A409-D987-4ADD-A716-3DFFDC350A6F}"/>
+    <hyperlink ref="B5" location="ZonaComun!A5" display="ZonaComun!A5" xr:uid="{30D63517-7BDF-4B21-AC86-26C0289B010C}"/>
+    <hyperlink ref="B6" location="ZonaComun!A6" display="ZonaComun!A6" xr:uid="{AC31C2F8-0C6A-4BA8-8A38-4A352EFB956B}"/>
+    <hyperlink ref="B7" location="ZonaComun!A4" display="ZonaComun!A4" xr:uid="{926F73C6-9695-42FB-9C89-7AD4F38DB238}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1293,30 +1355,30 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.109375" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="4" width="21.6640625" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" customWidth="1"/>
-    <col min="6" max="6" width="123.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="130.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="21.7109375" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" customWidth="1"/>
+    <col min="6" max="6" width="123.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="130.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="37" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>25</v>
       </c>
@@ -1337,7 +1399,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -1353,14 +1415,14 @@
       <c r="E3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <v>1</v>
       </c>
@@ -1376,19 +1438,19 @@
       <c r="E4" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="F4" s="15" t="str">
+      <c r="F4" s="41" t="str">
         <f>Agenda!$G$4</f>
-        <v>Agenda para residentes turno Diurno - 18  septiembre 2024 6:00:00 a. m.  hasta - 18  septiembre 2024 2:00:00 p. m. -Gimnasio-1-Forest apartamentos</v>
-      </c>
-      <c r="G4" s="16" t="str">
+        <v>Agenda para residentes turno Diurno - 18  septiembre 2024 6:00:00 a. m.  hasta - 18  septiembre 2024 2:00:00 p. m. -1-Forest apartamentos</v>
+      </c>
+      <c r="G4" s="15" t="str">
         <f t="shared" ref="G4:G21" si="0">_xlfn.CONCAT(B4,"-",F4)</f>
-        <v>Turno 1-Agenda para residentes turno Diurno - 18  septiembre 2024 6:00:00 a. m.  hasta - 18  septiembre 2024 2:00:00 p. m. -Gimnasio-1-Forest apartamentos</v>
+        <v>Turno 1-Agenda para residentes turno Diurno - 18  septiembre 2024 6:00:00 a. m.  hasta - 18  septiembre 2024 2:00:00 p. m. -1-Forest apartamentos</v>
       </c>
       <c r="I4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
         <v>2</v>
       </c>
@@ -1404,19 +1466,19 @@
       <c r="E5" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="F5" s="15" t="str">
+      <c r="F5" s="41" t="str">
         <f>Agenda!$G$4</f>
-        <v>Agenda para residentes turno Diurno - 18  septiembre 2024 6:00:00 a. m.  hasta - 18  septiembre 2024 2:00:00 p. m. -Gimnasio-1-Forest apartamentos</v>
-      </c>
-      <c r="G5" s="16" t="str">
+        <v>Agenda para residentes turno Diurno - 18  septiembre 2024 6:00:00 a. m.  hasta - 18  septiembre 2024 2:00:00 p. m. -1-Forest apartamentos</v>
+      </c>
+      <c r="G5" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>Turno 2-Agenda para residentes turno Diurno - 18  septiembre 2024 6:00:00 a. m.  hasta - 18  septiembre 2024 2:00:00 p. m. -Gimnasio-1-Forest apartamentos</v>
+        <v>Turno 2-Agenda para residentes turno Diurno - 18  septiembre 2024 6:00:00 a. m.  hasta - 18  septiembre 2024 2:00:00 p. m. -1-Forest apartamentos</v>
       </c>
       <c r="I5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
         <v>3</v>
       </c>
@@ -1432,19 +1494,19 @@
       <c r="E6" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="F6" s="15" t="str">
+      <c r="F6" s="41" t="str">
         <f>Agenda!$G$4</f>
-        <v>Agenda para residentes turno Diurno - 18  septiembre 2024 6:00:00 a. m.  hasta - 18  septiembre 2024 2:00:00 p. m. -Gimnasio-1-Forest apartamentos</v>
-      </c>
-      <c r="G6" s="16" t="str">
+        <v>Agenda para residentes turno Diurno - 18  septiembre 2024 6:00:00 a. m.  hasta - 18  septiembre 2024 2:00:00 p. m. -1-Forest apartamentos</v>
+      </c>
+      <c r="G6" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>Turno 3-Agenda para residentes turno Diurno - 18  septiembre 2024 6:00:00 a. m.  hasta - 18  septiembre 2024 2:00:00 p. m. -Gimnasio-1-Forest apartamentos</v>
+        <v>Turno 3-Agenda para residentes turno Diurno - 18  septiembre 2024 6:00:00 a. m.  hasta - 18  septiembre 2024 2:00:00 p. m. -1-Forest apartamentos</v>
       </c>
       <c r="I6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <v>4</v>
       </c>
@@ -1460,317 +1522,317 @@
       <c r="E7" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="F7" s="15" t="str">
+      <c r="F7" s="41" t="str">
         <f>Agenda!$G$4</f>
-        <v>Agenda para residentes turno Diurno - 18  septiembre 2024 6:00:00 a. m.  hasta - 18  septiembre 2024 2:00:00 p. m. -Gimnasio-1-Forest apartamentos</v>
-      </c>
-      <c r="G7" s="16" t="str">
+        <v>Agenda para residentes turno Diurno - 18  septiembre 2024 6:00:00 a. m.  hasta - 18  septiembre 2024 2:00:00 p. m. -1-Forest apartamentos</v>
+      </c>
+      <c r="G7" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>Turno 4-Agenda para residentes turno Diurno - 18  septiembre 2024 6:00:00 a. m.  hasta - 18  septiembre 2024 2:00:00 p. m. -Gimnasio-1-Forest apartamentos</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="17">
+        <v>Turno 4-Agenda para residentes turno Diurno - 18  septiembre 2024 6:00:00 a. m.  hasta - 18  septiembre 2024 2:00:00 p. m. -1-Forest apartamentos</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="16">
         <v>5</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="18">
+      <c r="C8" s="17">
         <v>0.625</v>
       </c>
-      <c r="D8" s="18">
+      <c r="D8" s="17">
         <v>0.70833333333333337</v>
       </c>
-      <c r="E8" s="19" t="s">
+      <c r="E8" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="20" t="str">
+      <c r="F8" s="42" t="str">
         <f>Agenda!$G$5</f>
-        <v>Agenda para residentes turno Nocturno - 18  septiembre 2024 3:00:00 p. m.  hasta - 18  septiembre 2024 9:00:00 p. m. -Gimnasio-1-Forest apartamentos</v>
-      </c>
-      <c r="G8" s="16" t="str">
+        <v>Agenda para residentes turno Nocturno - 18  septiembre 2024 3:00:00 p. m.  hasta - 18  septiembre 2024 9:00:00 p. m. -1-Forest apartamentos</v>
+      </c>
+      <c r="G8" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>Turno 1-Agenda para residentes turno Nocturno - 18  septiembre 2024 3:00:00 p. m.  hasta - 18  septiembre 2024 9:00:00 p. m. -Gimnasio-1-Forest apartamentos</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="17">
+        <v>Turno 1-Agenda para residentes turno Nocturno - 18  septiembre 2024 3:00:00 p. m.  hasta - 18  septiembre 2024 9:00:00 p. m. -1-Forest apartamentos</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="16">
         <v>6</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="18">
+      <c r="C9" s="17">
         <v>0.70833333333333337</v>
       </c>
-      <c r="D9" s="18">
+      <c r="D9" s="17">
         <v>0.79166666666666663</v>
       </c>
-      <c r="E9" s="19" t="s">
+      <c r="E9" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="F9" s="20" t="str">
+      <c r="F9" s="42" t="str">
         <f>Agenda!$G$5</f>
-        <v>Agenda para residentes turno Nocturno - 18  septiembre 2024 3:00:00 p. m.  hasta - 18  septiembre 2024 9:00:00 p. m. -Gimnasio-1-Forest apartamentos</v>
-      </c>
-      <c r="G9" s="16" t="str">
+        <v>Agenda para residentes turno Nocturno - 18  septiembre 2024 3:00:00 p. m.  hasta - 18  septiembre 2024 9:00:00 p. m. -1-Forest apartamentos</v>
+      </c>
+      <c r="G9" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>Turno 2-Agenda para residentes turno Nocturno - 18  septiembre 2024 3:00:00 p. m.  hasta - 18  septiembre 2024 9:00:00 p. m. -Gimnasio-1-Forest apartamentos</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="17">
+        <v>Turno 2-Agenda para residentes turno Nocturno - 18  septiembre 2024 3:00:00 p. m.  hasta - 18  septiembre 2024 9:00:00 p. m. -1-Forest apartamentos</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="16">
         <v>7</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="18">
+      <c r="C10" s="17">
         <v>0.79166666666666663</v>
       </c>
-      <c r="D10" s="18">
+      <c r="D10" s="17">
         <v>0.875</v>
       </c>
-      <c r="E10" s="19" t="s">
+      <c r="E10" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="F10" s="20" t="str">
+      <c r="F10" s="42" t="str">
         <f>Agenda!$G$5</f>
-        <v>Agenda para residentes turno Nocturno - 18  septiembre 2024 3:00:00 p. m.  hasta - 18  septiembre 2024 9:00:00 p. m. -Gimnasio-1-Forest apartamentos</v>
-      </c>
-      <c r="G10" s="16" t="str">
+        <v>Agenda para residentes turno Nocturno - 18  septiembre 2024 3:00:00 p. m.  hasta - 18  septiembre 2024 9:00:00 p. m. -1-Forest apartamentos</v>
+      </c>
+      <c r="G10" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>Turno 3-Agenda para residentes turno Nocturno - 18  septiembre 2024 3:00:00 p. m.  hasta - 18  septiembre 2024 9:00:00 p. m. -Gimnasio-1-Forest apartamentos</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="21">
+        <v>Turno 3-Agenda para residentes turno Nocturno - 18  septiembre 2024 3:00:00 p. m.  hasta - 18  septiembre 2024 9:00:00 p. m. -1-Forest apartamentos</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="19">
         <v>8</v>
       </c>
-      <c r="B11" s="21" t="s">
+      <c r="B11" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="22">
+      <c r="C11" s="20">
         <v>0.91666666666666663</v>
       </c>
-      <c r="D11" s="22">
+      <c r="D11" s="20">
         <v>0.95833333333333337</v>
       </c>
-      <c r="E11" s="23" t="s">
+      <c r="E11" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="F11" s="24" t="str">
+      <c r="F11" s="43" t="str">
         <f>Agenda!$G$6</f>
-        <v>Agenda para residentes - 20  septiembre 2024 10:00:00 a. m.  hasta - 20  septiembre 2024 1:00:00 p. m. -piscinaAdultos-2-Natural</v>
-      </c>
-      <c r="G11" s="16" t="str">
+        <v>Agenda para residentes - 20  septiembre 2024 10:00:00 a. m.  hasta - 20  septiembre 2024 1:00:00 p. m. -2-Natural</v>
+      </c>
+      <c r="G11" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>Turno 1-Agenda para residentes - 20  septiembre 2024 10:00:00 a. m.  hasta - 20  septiembre 2024 1:00:00 p. m. -piscinaAdultos-2-Natural</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="21">
+        <v>Turno 1-Agenda para residentes - 20  septiembre 2024 10:00:00 a. m.  hasta - 20  septiembre 2024 1:00:00 p. m. -2-Natural</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="19">
         <v>9</v>
       </c>
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="22">
+      <c r="C12" s="20">
         <v>0.45833333333333331</v>
       </c>
-      <c r="D12" s="22">
+      <c r="D12" s="20">
         <v>0.5</v>
       </c>
-      <c r="E12" s="23" t="s">
+      <c r="E12" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="F12" s="24" t="str">
+      <c r="F12" s="43" t="str">
         <f>Agenda!$G$6</f>
-        <v>Agenda para residentes - 20  septiembre 2024 10:00:00 a. m.  hasta - 20  septiembre 2024 1:00:00 p. m. -piscinaAdultos-2-Natural</v>
-      </c>
-      <c r="G12" s="16" t="str">
+        <v>Agenda para residentes - 20  septiembre 2024 10:00:00 a. m.  hasta - 20  septiembre 2024 1:00:00 p. m. -2-Natural</v>
+      </c>
+      <c r="G12" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>Turno 2-Agenda para residentes - 20  septiembre 2024 10:00:00 a. m.  hasta - 20  septiembre 2024 1:00:00 p. m. -piscinaAdultos-2-Natural</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="21">
+        <v>Turno 2-Agenda para residentes - 20  septiembre 2024 10:00:00 a. m.  hasta - 20  septiembre 2024 1:00:00 p. m. -2-Natural</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="19">
         <v>10</v>
       </c>
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="22">
+      <c r="C13" s="20">
         <v>0.5</v>
       </c>
-      <c r="D13" s="22">
+      <c r="D13" s="20">
         <v>0.54166666666666663</v>
       </c>
-      <c r="E13" s="23" t="s">
+      <c r="E13" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="F13" s="24" t="str">
+      <c r="F13" s="43" t="str">
         <f>Agenda!$G$6</f>
-        <v>Agenda para residentes - 20  septiembre 2024 10:00:00 a. m.  hasta - 20  septiembre 2024 1:00:00 p. m. -piscinaAdultos-2-Natural</v>
-      </c>
-      <c r="G13" s="16" t="str">
+        <v>Agenda para residentes - 20  septiembre 2024 10:00:00 a. m.  hasta - 20  septiembre 2024 1:00:00 p. m. -2-Natural</v>
+      </c>
+      <c r="G13" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>Turno 3-Agenda para residentes - 20  septiembre 2024 10:00:00 a. m.  hasta - 20  septiembre 2024 1:00:00 p. m. -piscinaAdultos-2-Natural</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="25">
+        <v>Turno 3-Agenda para residentes - 20  septiembre 2024 10:00:00 a. m.  hasta - 20  septiembre 2024 1:00:00 p. m. -2-Natural</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="22">
         <v>11</v>
       </c>
-      <c r="B14" s="25" t="s">
+      <c r="B14" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="26">
+      <c r="C14" s="23">
         <v>0.33333333333333331</v>
       </c>
-      <c r="D14" s="26">
+      <c r="D14" s="23">
         <v>0.375</v>
       </c>
-      <c r="E14" s="27" t="s">
+      <c r="E14" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="F14" s="28" t="str">
+      <c r="F14" s="44" t="str">
         <f>Agenda!$G$7</f>
-        <v>Agenda para dias de mantenimiento - 18  septiembre 2024 8:00:00 a. m.  hasta - 18  septiembre 2024 12:00:00 p. m. -Piscina-1-Forest apartamentos</v>
-      </c>
-      <c r="G14" s="16" t="str">
+        <v>Agenda para dias de mantenimiento - 18  septiembre 2024 8:00:00 a. m.  hasta - 18  septiembre 2024 12:00:00 p. m. -1-Forest apartamentos</v>
+      </c>
+      <c r="G14" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>Turno 1-Agenda para dias de mantenimiento - 18  septiembre 2024 8:00:00 a. m.  hasta - 18  septiembre 2024 12:00:00 p. m. -Piscina-1-Forest apartamentos</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="25">
+        <v>Turno 1-Agenda para dias de mantenimiento - 18  septiembre 2024 8:00:00 a. m.  hasta - 18  septiembre 2024 12:00:00 p. m. -1-Forest apartamentos</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="22">
         <v>12</v>
       </c>
-      <c r="B15" s="25" t="s">
+      <c r="B15" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="26">
+      <c r="C15" s="23">
         <v>0.375</v>
       </c>
-      <c r="D15" s="26">
+      <c r="D15" s="23">
         <v>0.41666666666666702</v>
       </c>
-      <c r="E15" s="27" t="s">
+      <c r="E15" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="F15" s="28" t="str">
+      <c r="F15" s="44" t="str">
         <f>Agenda!$G$7</f>
-        <v>Agenda para dias de mantenimiento - 18  septiembre 2024 8:00:00 a. m.  hasta - 18  septiembre 2024 12:00:00 p. m. -Piscina-1-Forest apartamentos</v>
-      </c>
-      <c r="G15" s="16" t="str">
+        <v>Agenda para dias de mantenimiento - 18  septiembre 2024 8:00:00 a. m.  hasta - 18  septiembre 2024 12:00:00 p. m. -1-Forest apartamentos</v>
+      </c>
+      <c r="G15" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>Turno 2-Agenda para dias de mantenimiento - 18  septiembre 2024 8:00:00 a. m.  hasta - 18  septiembre 2024 12:00:00 p. m. -Piscina-1-Forest apartamentos</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="25">
+        <v>Turno 2-Agenda para dias de mantenimiento - 18  septiembre 2024 8:00:00 a. m.  hasta - 18  septiembre 2024 12:00:00 p. m. -1-Forest apartamentos</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="22">
         <v>13</v>
       </c>
-      <c r="B16" s="25" t="s">
+      <c r="B16" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="26">
+      <c r="C16" s="23">
         <v>0.41666666666666702</v>
       </c>
-      <c r="D16" s="26">
+      <c r="D16" s="23">
         <v>0.45833333333333398</v>
       </c>
-      <c r="E16" s="27" t="s">
+      <c r="E16" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="F16" s="28" t="str">
+      <c r="F16" s="44" t="str">
         <f>Agenda!$G$7</f>
-        <v>Agenda para dias de mantenimiento - 18  septiembre 2024 8:00:00 a. m.  hasta - 18  septiembre 2024 12:00:00 p. m. -Piscina-1-Forest apartamentos</v>
-      </c>
-      <c r="G16" s="16" t="str">
+        <v>Agenda para dias de mantenimiento - 18  septiembre 2024 8:00:00 a. m.  hasta - 18  septiembre 2024 12:00:00 p. m. -1-Forest apartamentos</v>
+      </c>
+      <c r="G16" s="15" t="str">
         <f>_xlfn.CONCAT(B16,"-",F16)</f>
-        <v>Turno 3-Agenda para dias de mantenimiento - 18  septiembre 2024 8:00:00 a. m.  hasta - 18  septiembre 2024 12:00:00 p. m. -Piscina-1-Forest apartamentos</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="25">
+        <v>Turno 3-Agenda para dias de mantenimiento - 18  septiembre 2024 8:00:00 a. m.  hasta - 18  septiembre 2024 12:00:00 p. m. -1-Forest apartamentos</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="22">
         <v>14</v>
       </c>
-      <c r="B17" s="25" t="s">
+      <c r="B17" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="26">
+      <c r="C17" s="23">
         <v>0.45833333333333398</v>
       </c>
-      <c r="D17" s="26">
+      <c r="D17" s="23">
         <v>0.500000000000001</v>
       </c>
-      <c r="E17" s="27" t="s">
+      <c r="E17" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="F17" s="28" t="str">
+      <c r="F17" s="44" t="str">
         <f>Agenda!$G$7</f>
-        <v>Agenda para dias de mantenimiento - 18  septiembre 2024 8:00:00 a. m.  hasta - 18  septiembre 2024 12:00:00 p. m. -Piscina-1-Forest apartamentos</v>
-      </c>
-      <c r="G17" s="16" t="str">
+        <v>Agenda para dias de mantenimiento - 18  septiembre 2024 8:00:00 a. m.  hasta - 18  septiembre 2024 12:00:00 p. m. -1-Forest apartamentos</v>
+      </c>
+      <c r="G17" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>Turno 4-Agenda para dias de mantenimiento - 18  septiembre 2024 8:00:00 a. m.  hasta - 18  septiembre 2024 12:00:00 p. m. -Piscina-1-Forest apartamentos</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="29">
+        <v>Turno 4-Agenda para dias de mantenimiento - 18  septiembre 2024 8:00:00 a. m.  hasta - 18  septiembre 2024 12:00:00 p. m. -1-Forest apartamentos</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="25">
         <v>15</v>
       </c>
-      <c r="B18" s="29"/>
-      <c r="C18" s="30"/>
-      <c r="D18" s="30"/>
-      <c r="E18" s="31"/>
+      <c r="B18" s="25"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="27"/>
       <c r="F18" s="5"/>
-      <c r="G18" s="16" t="str">
+      <c r="G18" s="15" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="29">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="25">
         <v>16</v>
       </c>
-      <c r="B19" s="29"/>
-      <c r="C19" s="30"/>
-      <c r="D19" s="30"/>
-      <c r="E19" s="31"/>
+      <c r="B19" s="25"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="27"/>
       <c r="F19" s="5"/>
-      <c r="G19" s="16" t="str">
+      <c r="G19" s="15" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="29">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="25">
         <v>17</v>
       </c>
-      <c r="B20" s="29"/>
-      <c r="C20" s="30"/>
-      <c r="D20" s="30"/>
-      <c r="E20" s="31"/>
+      <c r="B20" s="25"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="27"/>
       <c r="F20" s="5"/>
-      <c r="G20" s="16" t="str">
+      <c r="G20" s="15" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="29">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="25">
         <v>18</v>
       </c>
-      <c r="B21" s="29"/>
-      <c r="C21" s="30"/>
-      <c r="D21" s="30"/>
-      <c r="E21" s="31"/>
+      <c r="B21" s="25"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="27"/>
       <c r="F21" s="5"/>
-      <c r="G21" s="16" t="str">
+      <c r="G21" s="15" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
@@ -1786,6 +1848,15 @@
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="A1" location="'Objetos de dominio'!A1" display="&lt;&lt;&lt;&lt;&lt;&lt; Volver al inicio" xr:uid="{3BFB3D8C-43E7-428F-8895-169BB452ED0C}"/>
+    <hyperlink ref="F3" location="Agenda!A1" display="Agenda" xr:uid="{782051DA-0D32-4E35-8074-1E45BE4AD18D}"/>
+    <hyperlink ref="F4" location="Agenda!A4" display="Agenda!A4" xr:uid="{0949AB94-0B3E-410A-B54E-D1E5CAECB10E}"/>
+    <hyperlink ref="F5:F7" location="Agenda!A4" display="Agenda!A4" xr:uid="{73A0B3CE-99AB-4E09-AF22-28798EDAFE81}"/>
+    <hyperlink ref="F8" location="Agenda!A5" display="Agenda!A5" xr:uid="{54052085-6879-4248-99F7-38A3197E355F}"/>
+    <hyperlink ref="F9:F10" location="Agenda!A5" display="Agenda!A5" xr:uid="{534D4E7B-15E9-4B1D-A0F2-A89B88A8CFEC}"/>
+    <hyperlink ref="F11" location="Agenda!A6" display="Agenda!A6" xr:uid="{E3DC0B23-33BD-4C6B-B995-6393382F6E80}"/>
+    <hyperlink ref="F12:F13" location="Agenda!A6" display="Agenda!A6" xr:uid="{80FC446E-D2D6-41BC-9038-C2D40ABFD613}"/>
+    <hyperlink ref="F14" location="Agenda!A7" display="Agenda!A7" xr:uid="{E07F057B-7AA2-4EB5-AA35-40FD6B814572}"/>
+    <hyperlink ref="F15:F17" location="Agenda!A7" display="Agenda!A7" xr:uid="{5B5095B4-5A47-4751-80A3-8121A3CB1B07}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Modelo enriquecido de agenda, hay que revisar parte de las combinaciones únicas y hacer la pregunta al profesor sobre cómo son estas.
</commit_message>
<xml_diff>
--- a/Doo-Doc/Nueva Version Victus/MuestreoDatos/Agenda Muestreo Datos.xlsx
+++ b/Doo-Doc/Nueva Version Victus/MuestreoDatos/Agenda Muestreo Datos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Music\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uconet-my.sharepoint.com/personal/juan_avendano1956_uco_net_co/Documents/Documents/victus-doc/Doo-Doc/Nueva Version Victus/MuestreoDatos/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B89AD7CE-8143-4AEB-B50A-6CDFA11B9B51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15855" yWindow="1725" windowWidth="20220" windowHeight="15345" activeTab="2" xr2:uid="{2D4B8DA6-DD27-486A-88C5-FC69C929F1D2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{2D4B8DA6-DD27-486A-88C5-FC69C929F1D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Objetos de dominio" sheetId="1" r:id="rId1"/>
@@ -479,7 +479,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -548,8 +548,12 @@
 </externalLink>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -871,13 +875,13 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" customWidth="1"/>
-    <col min="2" max="2" width="58.28515625" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" customWidth="1"/>
+    <col min="2" max="2" width="58.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -885,7 +889,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -893,7 +897,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -901,7 +905,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -927,18 +931,18 @@
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="21.7109375" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
     <col min="4" max="4" width="27" customWidth="1"/>
-    <col min="5" max="7" width="21.7109375" customWidth="1"/>
+    <col min="5" max="7" width="21.6640625" customWidth="1"/>
     <col min="8" max="8" width="15" customWidth="1"/>
-    <col min="9" max="9" width="23.7109375" customWidth="1"/>
-    <col min="10" max="10" width="33.140625" customWidth="1"/>
+    <col min="9" max="9" width="23.6640625" customWidth="1"/>
+    <col min="10" max="10" width="33.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="45" t="s">
         <v>7</v>
       </c>
@@ -952,7 +956,7 @@
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>42</v>
       </c>
@@ -980,7 +984,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -1012,7 +1016,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="76.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" ht="58.8" x14ac:dyDescent="0.4">
       <c r="A4" s="32">
         <v>1</v>
       </c>
@@ -1044,7 +1048,7 @@
         <v>Piscina-1-Forest apartamentos</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="84" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" ht="84" x14ac:dyDescent="0.4">
       <c r="A5" s="36">
         <v>2</v>
       </c>
@@ -1076,7 +1080,7 @@
         <v>Gimnasio-1-Forest apartamentos</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="76.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="58.8" x14ac:dyDescent="0.4">
       <c r="A6" s="36">
         <v>3</v>
       </c>
@@ -1124,21 +1128,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4578BD62-C112-42DC-9A20-08C85087F0AF}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="40.42578125" customWidth="1"/>
-    <col min="3" max="3" width="40.5703125" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" customWidth="1"/>
-    <col min="5" max="5" width="46.140625" customWidth="1"/>
-    <col min="6" max="6" width="44.7109375" customWidth="1"/>
-    <col min="7" max="7" width="128.42578125" customWidth="1"/>
+    <col min="2" max="2" width="40.44140625" customWidth="1"/>
+    <col min="3" max="3" width="40.5546875" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" customWidth="1"/>
+    <col min="5" max="5" width="46.109375" customWidth="1"/>
+    <col min="6" max="6" width="44.6640625" customWidth="1"/>
+    <col min="7" max="7" width="128.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="45" t="s">
         <v>7</v>
       </c>
@@ -1148,7 +1152,7 @@
       <c r="E1" s="45"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>8</v>
       </c>
@@ -1165,7 +1169,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -1188,7 +1192,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="9">
         <v>1</v>
       </c>
@@ -1213,7 +1217,7 @@
         <v>Agenda para residentes turno Diurno - 18  septiembre 2024 6:00:00 a. m.  hasta - 18  septiembre 2024 2:00:00 p. m. -1-Forest apartamentos</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="9">
         <v>2</v>
       </c>
@@ -1238,7 +1242,7 @@
         <v>Agenda para residentes turno Nocturno - 18  septiembre 2024 3:00:00 p. m.  hasta - 18  septiembre 2024 9:00:00 p. m. -1-Forest apartamentos</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="9">
         <v>3</v>
       </c>
@@ -1263,7 +1267,7 @@
         <v>Agenda para residentes - 20  septiembre 2024 10:00:00 a. m.  hasta - 20  septiembre 2024 1:00:00 p. m. -2-Natural</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="9">
         <v>4</v>
       </c>
@@ -1288,7 +1292,7 @@
         <v>Agenda para dias de mantenimiento - 18  septiembre 2024 8:00:00 a. m.  hasta - 18  septiembre 2024 12:00:00 p. m. -1-Forest apartamentos</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
       <c r="B8" s="10"/>
       <c r="C8" s="9"/>
@@ -1297,7 +1301,7 @@
       <c r="F8" s="11"/>
       <c r="G8" s="8"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="9"/>
       <c r="B9" s="10"/>
       <c r="C9" s="9"/>
@@ -1306,7 +1310,7 @@
       <c r="F9" s="11"/>
       <c r="G9" s="8"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
       <c r="B10" s="10"/>
       <c r="C10" s="5"/>
@@ -1315,7 +1319,7 @@
       <c r="F10" s="11"/>
       <c r="G10" s="8"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="9"/>
       <c r="B11" s="10"/>
       <c r="C11" s="5"/>
@@ -1324,12 +1328,12 @@
       <c r="F11" s="11"/>
       <c r="G11" s="8"/>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>24</v>
       </c>
@@ -1354,21 +1358,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1481DBD8-8614-460B-A4B3-0BC96282F835}">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="1" max="1" width="14.109375" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="4" width="21.7109375" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" customWidth="1"/>
-    <col min="6" max="6" width="123.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="130.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="21.6640625" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" customWidth="1"/>
+    <col min="6" max="6" width="123.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="130.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="45" t="s">
         <v>7</v>
       </c>
@@ -1378,7 +1382,7 @@
       <c r="E1" s="45"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>25</v>
       </c>
@@ -1399,7 +1403,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -1422,7 +1426,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="12">
         <v>1</v>
       </c>
@@ -1450,7 +1454,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="12">
         <v>2</v>
       </c>
@@ -1478,7 +1482,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="12">
         <v>3</v>
       </c>
@@ -1506,7 +1510,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="12">
         <v>4</v>
       </c>
@@ -1531,7 +1535,7 @@
         <v>Turno 4-Agenda para residentes turno Diurno - 18  septiembre 2024 6:00:00 a. m.  hasta - 18  septiembre 2024 2:00:00 p. m. -1-Forest apartamentos</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="16">
         <v>5</v>
       </c>
@@ -1556,7 +1560,7 @@
         <v>Turno 1-Agenda para residentes turno Nocturno - 18  septiembre 2024 3:00:00 p. m.  hasta - 18  septiembre 2024 9:00:00 p. m. -1-Forest apartamentos</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="16">
         <v>6</v>
       </c>
@@ -1581,7 +1585,7 @@
         <v>Turno 2-Agenda para residentes turno Nocturno - 18  septiembre 2024 3:00:00 p. m.  hasta - 18  septiembre 2024 9:00:00 p. m. -1-Forest apartamentos</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="16">
         <v>7</v>
       </c>
@@ -1606,7 +1610,7 @@
         <v>Turno 3-Agenda para residentes turno Nocturno - 18  septiembre 2024 3:00:00 p. m.  hasta - 18  septiembre 2024 9:00:00 p. m. -1-Forest apartamentos</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="19">
         <v>8</v>
       </c>
@@ -1631,7 +1635,7 @@
         <v>Turno 1-Agenda para residentes - 20  septiembre 2024 10:00:00 a. m.  hasta - 20  septiembre 2024 1:00:00 p. m. -2-Natural</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="19">
         <v>9</v>
       </c>
@@ -1656,7 +1660,7 @@
         <v>Turno 2-Agenda para residentes - 20  septiembre 2024 10:00:00 a. m.  hasta - 20  septiembre 2024 1:00:00 p. m. -2-Natural</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="19">
         <v>10</v>
       </c>
@@ -1681,7 +1685,7 @@
         <v>Turno 3-Agenda para residentes - 20  septiembre 2024 10:00:00 a. m.  hasta - 20  septiembre 2024 1:00:00 p. m. -2-Natural</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="22">
         <v>11</v>
       </c>
@@ -1706,7 +1710,7 @@
         <v>Turno 1-Agenda para dias de mantenimiento - 18  septiembre 2024 8:00:00 a. m.  hasta - 18  septiembre 2024 12:00:00 p. m. -1-Forest apartamentos</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="22">
         <v>12</v>
       </c>
@@ -1731,7 +1735,7 @@
         <v>Turno 2-Agenda para dias de mantenimiento - 18  septiembre 2024 8:00:00 a. m.  hasta - 18  septiembre 2024 12:00:00 p. m. -1-Forest apartamentos</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="22">
         <v>13</v>
       </c>
@@ -1756,7 +1760,7 @@
         <v>Turno 3-Agenda para dias de mantenimiento - 18  septiembre 2024 8:00:00 a. m.  hasta - 18  septiembre 2024 12:00:00 p. m. -1-Forest apartamentos</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="22">
         <v>14</v>
       </c>
@@ -1781,7 +1785,7 @@
         <v>Turno 4-Agenda para dias de mantenimiento - 18  septiembre 2024 8:00:00 a. m.  hasta - 18  septiembre 2024 12:00:00 p. m. -1-Forest apartamentos</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="25">
         <v>15</v>
       </c>
@@ -1795,7 +1799,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="25">
         <v>16</v>
       </c>
@@ -1809,7 +1813,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="25">
         <v>17</v>
       </c>
@@ -1823,7 +1827,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="25">
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
Faltan unas cositas en agenda
</commit_message>
<xml_diff>
--- a/Doo-Doc/Nueva Version Victus/MuestreoDatos/Agenda Muestreo Datos.xlsx
+++ b/Doo-Doc/Nueva Version Victus/MuestreoDatos/Agenda Muestreo Datos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uconet-my.sharepoint.com/personal/juan_avendano1956_uco_net_co/Documents/Documents/victus-doc/Doo-Doc/Nueva Version Victus/MuestreoDatos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B89AD7CE-8143-4AEB-B50A-6CDFA11B9B51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{B89AD7CE-8143-4AEB-B50A-6CDFA11B9B51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4A63616D-7A8A-4FD5-AAE1-35AFDD49DE25}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{2D4B8DA6-DD27-486A-88C5-FC69C929F1D2}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="93">
   <si>
     <t>Nombre</t>
   </si>
@@ -113,12 +113,6 @@
     <t>Agenda para dias de mantenimiento</t>
   </si>
   <si>
-    <t>dddd, d "de" mmmm "de" yyyy h:mm:ss AM/PM</t>
-  </si>
-  <si>
-    <t>Este es el formato personalizado que estamos usando</t>
-  </si>
-  <si>
     <t>Es un dato que hace que cada turno sea único.</t>
   </si>
   <si>
@@ -197,9 +191,6 @@
     <t>Imagen</t>
   </si>
   <si>
-    <t>Capacidad</t>
-  </si>
-  <si>
     <t>Normas</t>
   </si>
   <si>
@@ -233,16 +224,103 @@
     <t>Corresponde a los turnos que un residente puede reservar en una agenda, es decir, el residente toma un turno que esta disponible de una agenda que anteriormente ya esta programada.</t>
   </si>
   <si>
-    <t>tiempoUso</t>
-  </si>
-  <si>
-    <t>unidadDeTiempoUso</t>
-  </si>
-  <si>
     <t>Minutos</t>
   </si>
   <si>
     <t>Hora</t>
+  </si>
+  <si>
+    <t>Es un dato que representa cuantos minutos son permitidos por uso en un dia la zona común</t>
+  </si>
+  <si>
+    <t>Capacidad de personas</t>
+  </si>
+  <si>
+    <t>tiempo de uso</t>
+  </si>
+  <si>
+    <t>Unidad de tiempo de uso</t>
+  </si>
+  <si>
+    <t>piscina001.jpg</t>
+  </si>
+  <si>
+    <t>gimnasio002.jpg</t>
+  </si>
+  <si>
+    <t>piscinaadultos003.jpg</t>
+  </si>
+  <si>
+    <t>Salón de Eventos</t>
+  </si>
+  <si>
+    <t>salón de eventos004.jpg</t>
+  </si>
+  <si>
+    <t>Un espacio amplio para celebrar reuniones sociales y familiares.</t>
+  </si>
+  <si>
+    <t>Reservar con al menos 3 días de anticipación. No se permite el uso de pirotecnia.</t>
+  </si>
+  <si>
+    <t>Cancha de Fútbol</t>
+  </si>
+  <si>
+    <t>cancha de fútbol005.jpg</t>
+  </si>
+  <si>
+    <t>Cancha de césped sintético para actividades deportivas en equipo.</t>
+  </si>
+  <si>
+    <t>Se requiere reservar con 2 horas de anticipación. Uso exclusivo de zapatos con tacos adecuados.</t>
+  </si>
+  <si>
+    <t>Piscina Pequeña</t>
+  </si>
+  <si>
+    <t>piscina pequeña006.jpg</t>
+  </si>
+  <si>
+    <t>Piscina diseñada para niños, con profundidades seguras y vigilancia.</t>
+  </si>
+  <si>
+    <t>Es necesario el acompañamiento de un adulto. No se permite correr alrededor de la piscina.</t>
+  </si>
+  <si>
+    <t>Zona BBQ</t>
+  </si>
+  <si>
+    <t>zona bbq007.jpg</t>
+  </si>
+  <si>
+    <t>Área equipada con parrillas y mesas para realizar asados al aire libre.</t>
+  </si>
+  <si>
+    <t>Limpiar el área después de cada uso. Se debe reservar con 1 día de anticipación.</t>
+  </si>
+  <si>
+    <t>Cancha de Tenis</t>
+  </si>
+  <si>
+    <t>cancha de tenis008.jpg</t>
+  </si>
+  <si>
+    <t>Espacio deportivo para la práctica de tenis en un ambiente profesional</t>
+  </si>
+  <si>
+    <t>Uso exclusivo de zapatos de suela lisa. Reservar con 4 horas de anticipación.</t>
+  </si>
+  <si>
+    <t>Sala de Juegos</t>
+  </si>
+  <si>
+    <t>sala de juegos009.jpg</t>
+  </si>
+  <si>
+    <t>Sala equipada con mesas de ping-pong, billar y juegos de mesa para el disfrute familiar.</t>
+  </si>
+  <si>
+    <t>Reservar con al menos 2 horas de anticipación. Prohibido el consumo de alimentos en la sala.</t>
   </si>
 </sst>
 </file>
@@ -253,7 +331,7 @@
     <numFmt numFmtId="164" formatCode="dddd\,\ d\ &quot;de&quot;\ mmmm\ &quot;de&quot;\ yyyy\ h:mm:ss\ AM/PM"/>
     <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -287,28 +365,6 @@
     <font>
       <sz val="8"/>
       <color rgb="FF4EA72E"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="16"/>
-      <color rgb="FF000000"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="16"/>
-      <color theme="10"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="16"/>
-      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -392,7 +448,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -408,9 +464,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -436,37 +489,7 @@
     <xf numFmtId="165" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -476,6 +499,29 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -514,42 +560,37 @@
       <sheetData sheetId="1"/>
       <sheetData sheetId="2">
         <row r="4">
-          <cell r="G4" t="str">
-            <v>1-Forest apartamentos</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="G5" t="str">
-            <v>2-Natural</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5">
-        <row r="4">
           <cell r="I4" t="str">
             <v>1-Forest apartamentos</v>
           </cell>
         </row>
         <row r="5">
           <cell r="I5" t="str">
-            <v>1-Forest apartamentos</v>
+            <v>2-Natural</v>
           </cell>
         </row>
         <row r="6">
           <cell r="I6" t="str">
-            <v>2-Natural</v>
+            <v>3-Riogrande</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="I7" t="str">
+            <v>4-Bolivar</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="I8" t="str">
+            <v>5-Ventus</v>
           </cell>
         </row>
       </sheetData>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -902,7 +943,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -910,7 +951,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -925,16 +966,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AAB45A7-2401-4156-812B-1376902CA2CF}">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="21.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="3" max="3" width="24.6640625" customWidth="1"/>
     <col min="4" max="4" width="27" customWidth="1"/>
     <col min="5" max="7" width="21.6640625" customWidth="1"/>
     <col min="8" max="8" width="15" customWidth="1"/>
@@ -943,14 +984,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="31"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
       <c r="I1" s="6"/>
@@ -958,30 +999,32 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="D2" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="F2" s="7"/>
+      <c r="G2" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="H2" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="I2" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7" t="s">
+      <c r="J2" s="7" t="s">
         <v>47</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -992,133 +1035,361 @@
         <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="24" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="31">
+        <v>1</v>
+      </c>
+      <c r="B4" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="H3" s="1" t="s">
+      <c r="C4" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="I3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J3" s="28" t="s">
+      <c r="E4" s="31">
+        <v>50</v>
+      </c>
+      <c r="F4" s="31">
+        <v>60</v>
+      </c>
+      <c r="G4" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="58.8" x14ac:dyDescent="0.4">
-      <c r="A4" s="32">
-        <v>1</v>
-      </c>
-      <c r="B4" s="32" t="s">
-        <v>54</v>
-      </c>
-      <c r="C4" s="33"/>
-      <c r="D4" s="34" t="s">
-        <v>55</v>
-      </c>
-      <c r="E4" s="35">
-        <v>50</v>
-      </c>
-      <c r="F4" s="35">
-        <v>60</v>
-      </c>
-      <c r="G4" s="35" t="s">
-        <v>65</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="I4" s="25" t="str">
-        <f>[1]ConjuntoResidencial!$G$4</f>
+      <c r="I4" s="32" t="str">
+        <f>[1]ConjuntoResidencial!$I$4</f>
         <v>1-Forest apartamentos</v>
       </c>
-      <c r="J4" s="29" t="str">
+      <c r="J4" s="33" t="str">
         <f>_xlfn.CONCAT(B4,"-",I4)</f>
         <v>Piscina-1-Forest apartamentos</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="84" x14ac:dyDescent="0.4">
-      <c r="A5" s="36">
+    <row r="5" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="34">
         <v>2</v>
       </c>
-      <c r="B5" s="36" t="s">
-        <v>57</v>
-      </c>
-      <c r="C5" s="36"/>
-      <c r="D5" s="37" t="s">
-        <v>58</v>
-      </c>
-      <c r="E5" s="38">
+      <c r="B5" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="D5" s="35" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" s="34">
         <v>20</v>
       </c>
-      <c r="F5" s="38">
+      <c r="F5" s="34">
         <v>120</v>
       </c>
-      <c r="G5" s="38" t="s">
-        <v>65</v>
-      </c>
-      <c r="H5" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="I5" s="25" t="str">
-        <f>[1]ConjuntoResidencial!$G$4</f>
+      <c r="G5" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="H5" s="35" t="s">
+        <v>56</v>
+      </c>
+      <c r="I5" s="32" t="str">
+        <f>[1]ConjuntoResidencial!$I$4</f>
         <v>1-Forest apartamentos</v>
       </c>
-      <c r="J5" s="29" t="str">
+      <c r="J5" s="33" t="str">
         <f>_xlfn.CONCAT(B5,"-",I5)</f>
         <v>Gimnasio-1-Forest apartamentos</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="58.8" x14ac:dyDescent="0.4">
-      <c r="A6" s="36">
+    <row r="6" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="34">
         <v>3</v>
       </c>
-      <c r="B6" s="36" t="s">
-        <v>60</v>
-      </c>
-      <c r="C6" s="36"/>
-      <c r="D6" s="39" t="s">
-        <v>55</v>
-      </c>
-      <c r="E6" s="38">
+      <c r="B6" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" s="34">
         <v>15</v>
       </c>
-      <c r="F6" s="38">
+      <c r="F6" s="34">
         <v>1</v>
       </c>
-      <c r="G6" s="38" t="s">
-        <v>66</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="I6" s="25" t="str">
-        <f>[1]ConjuntoResidencial!$G$5</f>
+      <c r="G6" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="I6" s="32" t="str">
+        <f>[1]ConjuntoResidencial!$I$5</f>
         <v>2-Natural</v>
       </c>
-      <c r="J6" s="29" t="str">
+      <c r="J6" s="33" t="str">
         <f>_xlfn.CONCAT(B6,"-",I6)</f>
         <v>piscinaAdultos-2-Natural</v>
       </c>
     </row>
+    <row r="7" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+      <c r="A7" s="34">
+        <v>4</v>
+      </c>
+      <c r="B7" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="D7" s="35" t="s">
+        <v>71</v>
+      </c>
+      <c r="E7" s="34">
+        <v>100</v>
+      </c>
+      <c r="F7" s="34">
+        <v>4</v>
+      </c>
+      <c r="G7" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="H7" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="I7" s="32" t="str">
+        <f>[1]ConjuntoResidencial!I6</f>
+        <v>3-Riogrande</v>
+      </c>
+      <c r="J7" s="33" t="str">
+        <f t="shared" ref="J7:J12" si="0">_xlfn.CONCAT(B7,"-",I7)</f>
+        <v>Salón de Eventos-3-Riogrande</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="34">
+        <v>5</v>
+      </c>
+      <c r="B8" s="34" t="s">
+        <v>73</v>
+      </c>
+      <c r="C8" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="D8" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="E8" s="34">
+        <v>22</v>
+      </c>
+      <c r="F8" s="34">
+        <v>90</v>
+      </c>
+      <c r="G8" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="H8" s="35" t="s">
+        <v>76</v>
+      </c>
+      <c r="I8" s="32" t="str">
+        <f>[1]ConjuntoResidencial!I7</f>
+        <v>4-Bolivar</v>
+      </c>
+      <c r="J8" s="33" t="str">
+        <f t="shared" si="0"/>
+        <v>Cancha de Fútbol-4-Bolivar</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A9" s="34">
+        <v>6</v>
+      </c>
+      <c r="B9" s="34" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="D9" s="35" t="s">
+        <v>79</v>
+      </c>
+      <c r="E9" s="34">
+        <v>20</v>
+      </c>
+      <c r="F9" s="34">
+        <v>45</v>
+      </c>
+      <c r="G9" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="H9" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="I9" s="32" t="str">
+        <f>[1]ConjuntoResidencial!I5</f>
+        <v>2-Natural</v>
+      </c>
+      <c r="J9" s="33" t="str">
+        <f t="shared" si="0"/>
+        <v>Piscina Pequeña-2-Natural</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A10" s="34">
+        <v>7</v>
+      </c>
+      <c r="B10" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="C10" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="D10" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="E10" s="34">
+        <v>15</v>
+      </c>
+      <c r="F10" s="34">
+        <v>2</v>
+      </c>
+      <c r="G10" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="H10" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="I10" s="32" t="str">
+        <f>[1]ConjuntoResidencial!I8</f>
+        <v>5-Ventus</v>
+      </c>
+      <c r="J10" s="33" t="str">
+        <f t="shared" si="0"/>
+        <v>Zona BBQ-5-Ventus</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+      <c r="A11" s="34">
+        <v>8</v>
+      </c>
+      <c r="B11" s="34" t="s">
+        <v>85</v>
+      </c>
+      <c r="C11" s="32" t="s">
+        <v>86</v>
+      </c>
+      <c r="D11" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="E11" s="34">
+        <v>4</v>
+      </c>
+      <c r="F11" s="34">
+        <v>60</v>
+      </c>
+      <c r="G11" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="H11" s="35" t="s">
+        <v>88</v>
+      </c>
+      <c r="I11" s="32" t="str">
+        <f>[1]ConjuntoResidencial!I6</f>
+        <v>3-Riogrande</v>
+      </c>
+      <c r="J11" s="33" t="str">
+        <f t="shared" si="0"/>
+        <v>Cancha de Tenis-3-Riogrande</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="34">
+        <v>9</v>
+      </c>
+      <c r="B12" s="34" t="s">
+        <v>89</v>
+      </c>
+      <c r="C12" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="D12" s="35" t="s">
+        <v>91</v>
+      </c>
+      <c r="E12" s="34">
+        <v>10</v>
+      </c>
+      <c r="F12" s="34">
+        <v>90</v>
+      </c>
+      <c r="G12" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="H12" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="I12" s="32" t="str">
+        <f>[1]ConjuntoResidencial!I4</f>
+        <v>1-Forest apartamentos</v>
+      </c>
+      <c r="J12" s="33" t="str">
+        <f t="shared" si="0"/>
+        <v>Sala de Juegos-1-Forest apartamentos</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B13" s="36"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="38"/>
+      <c r="H13" s="38"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C14" s="37"/>
+      <c r="D14" s="38"/>
+      <c r="H14" s="38"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C15" s="37"/>
+      <c r="D15" s="38"/>
+      <c r="H15" s="38"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:E1"/>
-  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A1" location="'Objetos de dominio'!A1" display="&lt;&lt;&lt;&lt;&lt;&lt; Volver al inicio" xr:uid="{42E27472-290F-498E-8D59-E2019AE03564}"/>
-    <hyperlink ref="J1" location="Objetos de dominio!A1" display="Objetos de dominio!A1" xr:uid="{66BB4A93-8C9D-4AFA-80A4-F6947BF9E083}"/>
+    <hyperlink ref="A1" location="Objetos de dominio!A1" display="Objetos de dominio!A1" xr:uid="{CBEDEE6C-22FE-43B3-89F1-C741AF6805E9}"/>
+    <hyperlink ref="B1" location="Objetos de dominio!A1" display="Objetos de dominio!A1" xr:uid="{5049E57E-E139-4ADD-9C47-2609FB902FFB}"/>
+    <hyperlink ref="J1" location="Objetos de dominio!A1" display="Objetos de dominio!A1" xr:uid="{C8B3E4EF-57B4-4A4C-936C-454FCCF14785}"/>
+    <hyperlink ref="I3" location="ConjuntoResidencial!A1" display="ConjuntoResidencial" xr:uid="{FA68C03A-4D40-437E-A7E7-34175C992F59}"/>
+    <hyperlink ref="I4" location="ConjuntoResidencial!A5" display="ConjuntoResidencial!A5" xr:uid="{EB5BF42C-0DC8-4822-8A90-7F46EFD084D1}"/>
+    <hyperlink ref="I5" location="ConjuntoResidencial!A5" display="ConjuntoResidencial!A5" xr:uid="{50984DC8-E1AF-407A-A8DF-68C2FF5A2144}"/>
+    <hyperlink ref="I6" location="ConjuntoResidencial!A5" display="ConjuntoResidencial!A5" xr:uid="{BA2EDD1E-B40E-479F-88EC-DCC6DF46D04F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1126,10 +1397,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4578BD62-C112-42DC-9A20-08C85087F0AF}">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1143,13 +1414,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
       <c r="F1" s="6"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -1196,9 +1467,9 @@
       <c r="A4" s="9">
         <v>1</v>
       </c>
-      <c r="B4" s="40" t="str">
-        <f>[1]ZonaComun!$I$5</f>
-        <v>1-Forest apartamentos</v>
+      <c r="B4" s="25" t="str">
+        <f>ZonaComun!J4</f>
+        <v>Piscina-1-Forest apartamentos</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>18</v>
@@ -1206,24 +1477,24 @@
       <c r="D4" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="11">
+      <c r="E4" s="10">
         <v>45553.25</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F4" s="10">
         <v>45553.583333333336</v>
       </c>
       <c r="G4" s="8" t="str">
         <f>C4&amp;" "&amp;TEXT(E4,"- dd  mmmm yyyy h:mm:ss AM/PM ")&amp;" hasta "&amp;TEXT(F4,"- dd  mmmm yyyy h:mm:ss AM/PM ")&amp;"-"&amp;B4</f>
-        <v>Agenda para residentes turno Diurno - 18  septiembre 2024 6:00:00 a. m.  hasta - 18  septiembre 2024 2:00:00 p. m. -1-Forest apartamentos</v>
+        <v>Agenda para residentes turno Diurno - 18  septiembre 2024 6:00:00 a. m.  hasta - 18  septiembre 2024 2:00:00 p. m. -Piscina-1-Forest apartamentos</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="9">
         <v>2</v>
       </c>
-      <c r="B5" s="40" t="str">
-        <f>[1]ZonaComun!$I$5</f>
-        <v>1-Forest apartamentos</v>
+      <c r="B5" s="25" t="str">
+        <f>ZonaComun!J5</f>
+        <v>Gimnasio-1-Forest apartamentos</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>20</v>
@@ -1231,24 +1502,24 @@
       <c r="D5" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="11">
+      <c r="E5" s="10">
         <v>45553.625</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="10">
         <v>45553.875</v>
       </c>
       <c r="G5" s="8" t="str">
         <f t="shared" ref="G5:G7" si="0">C5&amp;" "&amp;TEXT(E5,"- dd  mmmm yyyy h:mm:ss AM/PM ")&amp;" hasta "&amp;TEXT(F5,"- dd  mmmm yyyy h:mm:ss AM/PM ")&amp;"-"&amp;B5</f>
-        <v>Agenda para residentes turno Nocturno - 18  septiembre 2024 3:00:00 p. m.  hasta - 18  septiembre 2024 9:00:00 p. m. -1-Forest apartamentos</v>
+        <v>Agenda para residentes turno Nocturno - 18  septiembre 2024 3:00:00 p. m.  hasta - 18  septiembre 2024 9:00:00 p. m. -Gimnasio-1-Forest apartamentos</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="9">
         <v>3</v>
       </c>
-      <c r="B6" s="40" t="str">
-        <f>[1]ZonaComun!$I$6</f>
-        <v>2-Natural</v>
+      <c r="B6" s="25" t="str">
+        <f>ZonaComun!J6</f>
+        <v>piscinaAdultos-2-Natural</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>21</v>
@@ -1256,24 +1527,24 @@
       <c r="D6" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="11">
+      <c r="E6" s="10">
         <v>45555.416666666664</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="10">
         <v>45555.541666666664</v>
       </c>
       <c r="G6" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>Agenda para residentes - 20  septiembre 2024 10:00:00 a. m.  hasta - 20  septiembre 2024 1:00:00 p. m. -2-Natural</v>
+        <v>Agenda para residentes - 20  septiembre 2024 10:00:00 a. m.  hasta - 20  septiembre 2024 1:00:00 p. m. -piscinaAdultos-2-Natural</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="9">
         <v>4</v>
       </c>
-      <c r="B7" s="40" t="str">
-        <f>[1]ZonaComun!$I$4</f>
-        <v>1-Forest apartamentos</v>
+      <c r="B7" s="25" t="str">
+        <f>ZonaComun!J7</f>
+        <v>Salón de Eventos-3-Riogrande</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>22</v>
@@ -1281,62 +1552,75 @@
       <c r="D7" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E7" s="10">
         <v>45553.333333333336</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="10">
         <v>45553.5</v>
       </c>
       <c r="G7" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>Agenda para dias de mantenimiento - 18  septiembre 2024 8:00:00 a. m.  hasta - 18  septiembre 2024 12:00:00 p. m. -1-Forest apartamentos</v>
+        <v>Agenda para dias de mantenimiento - 18  septiembre 2024 8:00:00 a. m.  hasta - 18  septiembre 2024 12:00:00 p. m. -Salón de Eventos-3-Riogrande</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="5"/>
-      <c r="B8" s="10"/>
+      <c r="A8" s="9">
+        <v>5</v>
+      </c>
+      <c r="B8" s="25" t="str">
+        <f>ZonaComun!J8</f>
+        <v>Cancha de Fútbol-4-Bolivar</v>
+      </c>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
       <c r="G8" s="8"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="9"/>
-      <c r="B9" s="10"/>
+      <c r="A9" s="9">
+        <v>6</v>
+      </c>
+      <c r="B9" s="25" t="str">
+        <f>ZonaComun!J9</f>
+        <v>Piscina Pequeña-2-Natural</v>
+      </c>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
       <c r="G9" s="8"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="5"/>
-      <c r="B10" s="10"/>
+      <c r="A10" s="9">
+        <v>7</v>
+      </c>
+      <c r="B10" s="25" t="str">
+        <f>ZonaComun!J10</f>
+        <v>Zona BBQ-5-Ventus</v>
+      </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
       <c r="G10" s="8"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="9"/>
-      <c r="B11" s="10"/>
+      <c r="A11" s="9">
+        <v>8</v>
+      </c>
+      <c r="B11" s="25" t="str">
+        <f>ZonaComun!J11</f>
+        <v>Cancha de Tenis-3-Riogrande</v>
+      </c>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
       <c r="G11" s="8"/>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B17" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B18" t="s">
-        <v>24</v>
-      </c>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1346,9 +1630,7 @@
     <hyperlink ref="A1" location="'Objetos de dominio'!A1" display="&lt;&lt;&lt;&lt;&lt;&lt; Volver al inicio" xr:uid="{80B0E295-9C45-4B66-99DF-E7CF9E9791FC}"/>
     <hyperlink ref="B3" location="ZonaComun!A1" display="ZonaComun" xr:uid="{23A414B0-B4D1-4009-AD81-8FE561EAB17A}"/>
     <hyperlink ref="B4" location="ZonaComun!A5" display="ZonaComun!A5" xr:uid="{0759A409-D987-4ADD-A716-3DFFDC350A6F}"/>
-    <hyperlink ref="B5" location="ZonaComun!A5" display="ZonaComun!A5" xr:uid="{30D63517-7BDF-4B21-AC86-26C0289B010C}"/>
-    <hyperlink ref="B6" location="ZonaComun!A6" display="ZonaComun!A6" xr:uid="{AC31C2F8-0C6A-4BA8-8A38-4A352EFB956B}"/>
-    <hyperlink ref="B7" location="ZonaComun!A4" display="ZonaComun!A4" xr:uid="{926F73C6-9695-42FB-9C89-7AD4F38DB238}"/>
+    <hyperlink ref="B5:B11" location="ZonaComun!A5" display="ZonaComun!A5" xr:uid="{EF8A20CE-7173-46C0-8D04-5DE6A0768865}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1356,10 +1638,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1481DBD8-8614-460B-A4B3-0BC96282F835}">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1373,34 +1655,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
       <c r="F1" s="6"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="D2" s="7" t="s">
         <v>26</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>28</v>
       </c>
       <c r="E2" s="7"/>
       <c r="F2" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -1408,16 +1690,16 @@
         <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>5</v>
@@ -1427,418 +1709,362 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="12">
+      <c r="A4" s="11">
         <v>1</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="12">
+        <v>0.25</v>
+      </c>
+      <c r="D4" s="12">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" s="26" t="str">
+        <f>Agenda!$G$4</f>
+        <v>Agenda para residentes turno Diurno - 18  septiembre 2024 6:00:00 a. m.  hasta - 18  septiembre 2024 2:00:00 p. m. -Piscina-1-Forest apartamentos</v>
+      </c>
+      <c r="G4" s="14" t="str">
+        <f t="shared" ref="G4:G21" si="0">_xlfn.CONCAT(B4,"-",F4)</f>
+        <v>Turno 1-Agenda para residentes turno Diurno - 18  septiembre 2024 6:00:00 a. m.  hasta - 18  septiembre 2024 2:00:00 p. m. -Piscina-1-Forest apartamentos</v>
+      </c>
+      <c r="I4" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="13">
-        <v>0.25</v>
-      </c>
-      <c r="D4" s="13">
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="11">
+        <v>2</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="12">
         <v>0.33333333333333331</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="D5" s="12">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" s="26" t="str">
+        <f>Agenda!$G$4</f>
+        <v>Agenda para residentes turno Diurno - 18  septiembre 2024 6:00:00 a. m.  hasta - 18  septiembre 2024 2:00:00 p. m. -Piscina-1-Forest apartamentos</v>
+      </c>
+      <c r="G5" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>Turno 2-Agenda para residentes turno Diurno - 18  septiembre 2024 6:00:00 a. m.  hasta - 18  septiembre 2024 2:00:00 p. m. -Piscina-1-Forest apartamentos</v>
+      </c>
+      <c r="I5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="11">
+        <v>3</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="12">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D6" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="26" t="str">
+        <f>Agenda!$G$4</f>
+        <v>Agenda para residentes turno Diurno - 18  septiembre 2024 6:00:00 a. m.  hasta - 18  septiembre 2024 2:00:00 p. m. -Piscina-1-Forest apartamentos</v>
+      </c>
+      <c r="G6" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>Turno 3-Agenda para residentes turno Diurno - 18  septiembre 2024 6:00:00 a. m.  hasta - 18  septiembre 2024 2:00:00 p. m. -Piscina-1-Forest apartamentos</v>
+      </c>
+      <c r="I6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="11">
+        <v>4</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="12">
+        <v>0.54166666666666696</v>
+      </c>
+      <c r="D7" s="12">
+        <v>0.58333333333333404</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="26" t="str">
+        <f>Agenda!$G$4</f>
+        <v>Agenda para residentes turno Diurno - 18  septiembre 2024 6:00:00 a. m.  hasta - 18  septiembre 2024 2:00:00 p. m. -Piscina-1-Forest apartamentos</v>
+      </c>
+      <c r="G7" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>Turno 4-Agenda para residentes turno Diurno - 18  septiembre 2024 6:00:00 a. m.  hasta - 18  septiembre 2024 2:00:00 p. m. -Piscina-1-Forest apartamentos</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="15">
+        <v>5</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="16">
+        <v>0.625</v>
+      </c>
+      <c r="D8" s="16">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" s="27" t="str">
+        <f>Agenda!$G$5</f>
+        <v>Agenda para residentes turno Nocturno - 18  septiembre 2024 3:00:00 p. m.  hasta - 18  septiembre 2024 9:00:00 p. m. -Gimnasio-1-Forest apartamentos</v>
+      </c>
+      <c r="G8" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>Turno 1-Agenda para residentes turno Nocturno - 18  septiembre 2024 3:00:00 p. m.  hasta - 18  septiembre 2024 9:00:00 p. m. -Gimnasio-1-Forest apartamentos</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="15">
+        <v>6</v>
+      </c>
+      <c r="B9" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="F4" s="41" t="str">
-        <f>Agenda!$G$4</f>
-        <v>Agenda para residentes turno Diurno - 18  septiembre 2024 6:00:00 a. m.  hasta - 18  septiembre 2024 2:00:00 p. m. -1-Forest apartamentos</v>
-      </c>
-      <c r="G4" s="15" t="str">
-        <f t="shared" ref="G4:G21" si="0">_xlfn.CONCAT(B4,"-",F4)</f>
-        <v>Turno 1-Agenda para residentes turno Diurno - 18  septiembre 2024 6:00:00 a. m.  hasta - 18  septiembre 2024 2:00:00 p. m. -1-Forest apartamentos</v>
-      </c>
-      <c r="I4" t="s">
+      <c r="C9" s="16">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D9" s="16">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" s="27" t="str">
+        <f>Agenda!$G$5</f>
+        <v>Agenda para residentes turno Nocturno - 18  septiembre 2024 3:00:00 p. m.  hasta - 18  septiembre 2024 9:00:00 p. m. -Gimnasio-1-Forest apartamentos</v>
+      </c>
+      <c r="G9" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>Turno 2-Agenda para residentes turno Nocturno - 18  septiembre 2024 3:00:00 p. m.  hasta - 18  septiembre 2024 9:00:00 p. m. -Gimnasio-1-Forest apartamentos</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="15">
+        <v>7</v>
+      </c>
+      <c r="B10" s="15" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="12">
-        <v>2</v>
-      </c>
-      <c r="B5" s="12" t="s">
+      <c r="C10" s="16">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="D10" s="16">
+        <v>0.875</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="27" t="str">
+        <f>Agenda!$G$5</f>
+        <v>Agenda para residentes turno Nocturno - 18  septiembre 2024 3:00:00 p. m.  hasta - 18  septiembre 2024 9:00:00 p. m. -Gimnasio-1-Forest apartamentos</v>
+      </c>
+      <c r="G10" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>Turno 3-Agenda para residentes turno Nocturno - 18  septiembre 2024 3:00:00 p. m.  hasta - 18  septiembre 2024 9:00:00 p. m. -Gimnasio-1-Forest apartamentos</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="18">
+        <v>8</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="19">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="D11" s="19">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="28" t="str">
+        <f>Agenda!$G$6</f>
+        <v>Agenda para residentes - 20  septiembre 2024 10:00:00 a. m.  hasta - 20  septiembre 2024 1:00:00 p. m. -piscinaAdultos-2-Natural</v>
+      </c>
+      <c r="G11" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>Turno 1-Agenda para residentes - 20  septiembre 2024 10:00:00 a. m.  hasta - 20  septiembre 2024 1:00:00 p. m. -piscinaAdultos-2-Natural</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="18">
+        <v>9</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="19">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D12" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" s="28" t="str">
+        <f>Agenda!$G$6</f>
+        <v>Agenda para residentes - 20  septiembre 2024 10:00:00 a. m.  hasta - 20  septiembre 2024 1:00:00 p. m. -piscinaAdultos-2-Natural</v>
+      </c>
+      <c r="G12" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>Turno 2-Agenda para residentes - 20  septiembre 2024 10:00:00 a. m.  hasta - 20  septiembre 2024 1:00:00 p. m. -piscinaAdultos-2-Natural</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="18">
+        <v>10</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="D13" s="19">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13" s="28" t="str">
+        <f>Agenda!$G$6</f>
+        <v>Agenda para residentes - 20  septiembre 2024 10:00:00 a. m.  hasta - 20  septiembre 2024 1:00:00 p. m. -piscinaAdultos-2-Natural</v>
+      </c>
+      <c r="G13" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>Turno 3-Agenda para residentes - 20  septiembre 2024 10:00:00 a. m.  hasta - 20  septiembre 2024 1:00:00 p. m. -piscinaAdultos-2-Natural</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="21">
+        <v>11</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="22">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D14" s="22">
+        <v>0.375</v>
+      </c>
+      <c r="E14" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="13">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="D5" s="13">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="E5" s="14" t="s">
+      <c r="F14" s="29" t="str">
+        <f>Agenda!$G$7</f>
+        <v>Agenda para dias de mantenimiento - 18  septiembre 2024 8:00:00 a. m.  hasta - 18  septiembre 2024 12:00:00 p. m. -Salón de Eventos-3-Riogrande</v>
+      </c>
+      <c r="G14" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>Turno 1-Agenda para dias de mantenimiento - 18  septiembre 2024 8:00:00 a. m.  hasta - 18  septiembre 2024 12:00:00 p. m. -Salón de Eventos-3-Riogrande</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="21">
+        <v>12</v>
+      </c>
+      <c r="B15" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="F5" s="41" t="str">
-        <f>Agenda!$G$4</f>
-        <v>Agenda para residentes turno Diurno - 18  septiembre 2024 6:00:00 a. m.  hasta - 18  septiembre 2024 2:00:00 p. m. -1-Forest apartamentos</v>
-      </c>
-      <c r="G5" s="15" t="str">
+      <c r="C15" s="22">
+        <v>0.375</v>
+      </c>
+      <c r="D15" s="22">
+        <v>0.41666666666666702</v>
+      </c>
+      <c r="E15" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="F15" s="29" t="str">
+        <f>Agenda!$G$7</f>
+        <v>Agenda para dias de mantenimiento - 18  septiembre 2024 8:00:00 a. m.  hasta - 18  septiembre 2024 12:00:00 p. m. -Salón de Eventos-3-Riogrande</v>
+      </c>
+      <c r="G15" s="14" t="str">
         <f t="shared" si="0"/>
-        <v>Turno 2-Agenda para residentes turno Diurno - 18  septiembre 2024 6:00:00 a. m.  hasta - 18  septiembre 2024 2:00:00 p. m. -1-Forest apartamentos</v>
-      </c>
-      <c r="I5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="12">
-        <v>3</v>
-      </c>
-      <c r="B6" s="12" t="s">
+        <v>Turno 2-Agenda para dias de mantenimiento - 18  septiembre 2024 8:00:00 a. m.  hasta - 18  septiembre 2024 12:00:00 p. m. -Salón de Eventos-3-Riogrande</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="21">
+        <v>13</v>
+      </c>
+      <c r="B16" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="22">
+        <v>0.41666666666666702</v>
+      </c>
+      <c r="D16" s="22">
+        <v>0.45833333333333398</v>
+      </c>
+      <c r="E16" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="F16" s="29" t="str">
+        <f>Agenda!$G$7</f>
+        <v>Agenda para dias de mantenimiento - 18  septiembre 2024 8:00:00 a. m.  hasta - 18  septiembre 2024 12:00:00 p. m. -Salón de Eventos-3-Riogrande</v>
+      </c>
+      <c r="G16" s="14" t="str">
+        <f>_xlfn.CONCAT(B16,"-",F16)</f>
+        <v>Turno 3-Agenda para dias de mantenimiento - 18  septiembre 2024 8:00:00 a. m.  hasta - 18  septiembre 2024 12:00:00 p. m. -Salón de Eventos-3-Riogrande</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="21">
+        <v>14</v>
+      </c>
+      <c r="B17" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="13">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="D6" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="E6" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="F6" s="41" t="str">
-        <f>Agenda!$G$4</f>
-        <v>Agenda para residentes turno Diurno - 18  septiembre 2024 6:00:00 a. m.  hasta - 18  septiembre 2024 2:00:00 p. m. -1-Forest apartamentos</v>
-      </c>
-      <c r="G6" s="15" t="str">
+      <c r="C17" s="22">
+        <v>0.45833333333333398</v>
+      </c>
+      <c r="D17" s="22">
+        <v>0.500000000000001</v>
+      </c>
+      <c r="E17" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="F17" s="29" t="str">
+        <f>Agenda!$G$7</f>
+        <v>Agenda para dias de mantenimiento - 18  septiembre 2024 8:00:00 a. m.  hasta - 18  septiembre 2024 12:00:00 p. m. -Salón de Eventos-3-Riogrande</v>
+      </c>
+      <c r="G17" s="14" t="str">
         <f t="shared" si="0"/>
-        <v>Turno 3-Agenda para residentes turno Diurno - 18  septiembre 2024 6:00:00 a. m.  hasta - 18  septiembre 2024 2:00:00 p. m. -1-Forest apartamentos</v>
-      </c>
-      <c r="I6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="12">
-        <v>4</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C7" s="13">
-        <v>0.54166666666666696</v>
-      </c>
-      <c r="D7" s="13">
-        <v>0.58333333333333404</v>
-      </c>
-      <c r="E7" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="F7" s="41" t="str">
-        <f>Agenda!$G$4</f>
-        <v>Agenda para residentes turno Diurno - 18  septiembre 2024 6:00:00 a. m.  hasta - 18  septiembre 2024 2:00:00 p. m. -1-Forest apartamentos</v>
-      </c>
-      <c r="G7" s="15" t="str">
-        <f t="shared" si="0"/>
-        <v>Turno 4-Agenda para residentes turno Diurno - 18  septiembre 2024 6:00:00 a. m.  hasta - 18  septiembre 2024 2:00:00 p. m. -1-Forest apartamentos</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="16">
-        <v>5</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" s="17">
-        <v>0.625</v>
-      </c>
-      <c r="D8" s="17">
-        <v>0.70833333333333337</v>
-      </c>
-      <c r="E8" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="F8" s="42" t="str">
-        <f>Agenda!$G$5</f>
-        <v>Agenda para residentes turno Nocturno - 18  septiembre 2024 3:00:00 p. m.  hasta - 18  septiembre 2024 9:00:00 p. m. -1-Forest apartamentos</v>
-      </c>
-      <c r="G8" s="15" t="str">
-        <f t="shared" si="0"/>
-        <v>Turno 1-Agenda para residentes turno Nocturno - 18  septiembre 2024 3:00:00 p. m.  hasta - 18  septiembre 2024 9:00:00 p. m. -1-Forest apartamentos</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="16">
-        <v>6</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" s="17">
-        <v>0.70833333333333337</v>
-      </c>
-      <c r="D9" s="17">
-        <v>0.79166666666666663</v>
-      </c>
-      <c r="E9" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="F9" s="42" t="str">
-        <f>Agenda!$G$5</f>
-        <v>Agenda para residentes turno Nocturno - 18  septiembre 2024 3:00:00 p. m.  hasta - 18  septiembre 2024 9:00:00 p. m. -1-Forest apartamentos</v>
-      </c>
-      <c r="G9" s="15" t="str">
-        <f t="shared" si="0"/>
-        <v>Turno 2-Agenda para residentes turno Nocturno - 18  septiembre 2024 3:00:00 p. m.  hasta - 18  septiembre 2024 9:00:00 p. m. -1-Forest apartamentos</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="16">
-        <v>7</v>
-      </c>
-      <c r="B10" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" s="17">
-        <v>0.79166666666666663</v>
-      </c>
-      <c r="D10" s="17">
-        <v>0.875</v>
-      </c>
-      <c r="E10" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="F10" s="42" t="str">
-        <f>Agenda!$G$5</f>
-        <v>Agenda para residentes turno Nocturno - 18  septiembre 2024 3:00:00 p. m.  hasta - 18  septiembre 2024 9:00:00 p. m. -1-Forest apartamentos</v>
-      </c>
-      <c r="G10" s="15" t="str">
-        <f t="shared" si="0"/>
-        <v>Turno 3-Agenda para residentes turno Nocturno - 18  septiembre 2024 3:00:00 p. m.  hasta - 18  septiembre 2024 9:00:00 p. m. -1-Forest apartamentos</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="19">
-        <v>8</v>
-      </c>
-      <c r="B11" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" s="20">
-        <v>0.91666666666666663</v>
-      </c>
-      <c r="D11" s="20">
-        <v>0.95833333333333337</v>
-      </c>
-      <c r="E11" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="F11" s="43" t="str">
-        <f>Agenda!$G$6</f>
-        <v>Agenda para residentes - 20  septiembre 2024 10:00:00 a. m.  hasta - 20  septiembre 2024 1:00:00 p. m. -2-Natural</v>
-      </c>
-      <c r="G11" s="15" t="str">
-        <f t="shared" si="0"/>
-        <v>Turno 1-Agenda para residentes - 20  septiembre 2024 10:00:00 a. m.  hasta - 20  septiembre 2024 1:00:00 p. m. -2-Natural</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="19">
-        <v>9</v>
-      </c>
-      <c r="B12" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="C12" s="20">
-        <v>0.45833333333333331</v>
-      </c>
-      <c r="D12" s="20">
-        <v>0.5</v>
-      </c>
-      <c r="E12" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="F12" s="43" t="str">
-        <f>Agenda!$G$6</f>
-        <v>Agenda para residentes - 20  septiembre 2024 10:00:00 a. m.  hasta - 20  septiembre 2024 1:00:00 p. m. -2-Natural</v>
-      </c>
-      <c r="G12" s="15" t="str">
-        <f t="shared" si="0"/>
-        <v>Turno 2-Agenda para residentes - 20  septiembre 2024 10:00:00 a. m.  hasta - 20  septiembre 2024 1:00:00 p. m. -2-Natural</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="19">
-        <v>10</v>
-      </c>
-      <c r="B13" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" s="20">
-        <v>0.5</v>
-      </c>
-      <c r="D13" s="20">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="E13" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="F13" s="43" t="str">
-        <f>Agenda!$G$6</f>
-        <v>Agenda para residentes - 20  septiembre 2024 10:00:00 a. m.  hasta - 20  septiembre 2024 1:00:00 p. m. -2-Natural</v>
-      </c>
-      <c r="G13" s="15" t="str">
-        <f t="shared" si="0"/>
-        <v>Turno 3-Agenda para residentes - 20  septiembre 2024 10:00:00 a. m.  hasta - 20  septiembre 2024 1:00:00 p. m. -2-Natural</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="22">
-        <v>11</v>
-      </c>
-      <c r="B14" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14" s="23">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="D14" s="23">
-        <v>0.375</v>
-      </c>
-      <c r="E14" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="F14" s="44" t="str">
-        <f>Agenda!$G$7</f>
-        <v>Agenda para dias de mantenimiento - 18  septiembre 2024 8:00:00 a. m.  hasta - 18  septiembre 2024 12:00:00 p. m. -1-Forest apartamentos</v>
-      </c>
-      <c r="G14" s="15" t="str">
-        <f t="shared" si="0"/>
-        <v>Turno 1-Agenda para dias de mantenimiento - 18  septiembre 2024 8:00:00 a. m.  hasta - 18  septiembre 2024 12:00:00 p. m. -1-Forest apartamentos</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="22">
-        <v>12</v>
-      </c>
-      <c r="B15" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="C15" s="23">
-        <v>0.375</v>
-      </c>
-      <c r="D15" s="23">
-        <v>0.41666666666666702</v>
-      </c>
-      <c r="E15" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="F15" s="44" t="str">
-        <f>Agenda!$G$7</f>
-        <v>Agenda para dias de mantenimiento - 18  septiembre 2024 8:00:00 a. m.  hasta - 18  septiembre 2024 12:00:00 p. m. -1-Forest apartamentos</v>
-      </c>
-      <c r="G15" s="15" t="str">
-        <f t="shared" si="0"/>
-        <v>Turno 2-Agenda para dias de mantenimiento - 18  septiembre 2024 8:00:00 a. m.  hasta - 18  septiembre 2024 12:00:00 p. m. -1-Forest apartamentos</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="22">
-        <v>13</v>
-      </c>
-      <c r="B16" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="C16" s="23">
-        <v>0.41666666666666702</v>
-      </c>
-      <c r="D16" s="23">
-        <v>0.45833333333333398</v>
-      </c>
-      <c r="E16" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="F16" s="44" t="str">
-        <f>Agenda!$G$7</f>
-        <v>Agenda para dias de mantenimiento - 18  septiembre 2024 8:00:00 a. m.  hasta - 18  septiembre 2024 12:00:00 p. m. -1-Forest apartamentos</v>
-      </c>
-      <c r="G16" s="15" t="str">
-        <f>_xlfn.CONCAT(B16,"-",F16)</f>
-        <v>Turno 3-Agenda para dias de mantenimiento - 18  septiembre 2024 8:00:00 a. m.  hasta - 18  septiembre 2024 12:00:00 p. m. -1-Forest apartamentos</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="22">
-        <v>14</v>
-      </c>
-      <c r="B17" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="C17" s="23">
-        <v>0.45833333333333398</v>
-      </c>
-      <c r="D17" s="23">
-        <v>0.500000000000001</v>
-      </c>
-      <c r="E17" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="F17" s="44" t="str">
-        <f>Agenda!$G$7</f>
-        <v>Agenda para dias de mantenimiento - 18  septiembre 2024 8:00:00 a. m.  hasta - 18  septiembre 2024 12:00:00 p. m. -1-Forest apartamentos</v>
-      </c>
-      <c r="G17" s="15" t="str">
-        <f t="shared" si="0"/>
-        <v>Turno 4-Agenda para dias de mantenimiento - 18  septiembre 2024 8:00:00 a. m.  hasta - 18  septiembre 2024 12:00:00 p. m. -1-Forest apartamentos</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="25">
-        <v>15</v>
-      </c>
-      <c r="B18" s="25"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="15" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="25">
-        <v>16</v>
-      </c>
-      <c r="B19" s="25"/>
-      <c r="C19" s="26"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="27"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="15" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="25">
-        <v>17</v>
-      </c>
-      <c r="B20" s="25"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="27"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="15" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="25">
-        <v>18</v>
-      </c>
-      <c r="B21" s="25"/>
-      <c r="C21" s="26"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="15" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <v>Turno 4-Agenda para dias de mantenimiento - 18  septiembre 2024 8:00:00 a. m.  hasta - 18  septiembre 2024 12:00:00 p. m. -Salón de Eventos-3-Riogrande</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Event storming de conjuntos residenciales y agendas ya separado adecuadamente además de creadas las entidades faltantes
</commit_message>
<xml_diff>
--- a/Doo-Doc/Nueva Version Victus/MuestreoDatos/Agenda Muestreo Datos.xlsx
+++ b/Doo-Doc/Nueva Version Victus/MuestreoDatos/Agenda Muestreo Datos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uconet-my.sharepoint.com/personal/juan_avendano1956_uco_net_co/Documents/Documents/victus-doc/Doo-Doc/Nueva Version Victus/MuestreoDatos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{B89AD7CE-8143-4AEB-B50A-6CDFA11B9B51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4A63616D-7A8A-4FD5-AAE1-35AFDD49DE25}"/>
+  <xr:revisionPtr revIDLastSave="35" documentId="13_ncr:1_{B89AD7CE-8143-4AEB-B50A-6CDFA11B9B51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AC8BE659-C693-4555-B61F-C0A10C7A817C}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{2D4B8DA6-DD27-486A-88C5-FC69C929F1D2}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="102">
   <si>
     <t>Nombre</t>
   </si>
@@ -101,9 +101,6 @@
     <t>Agenda para residentes turno Diurno</t>
   </si>
   <si>
-    <t>si</t>
-  </si>
-  <si>
     <t>Agenda para residentes turno Nocturno</t>
   </si>
   <si>
@@ -321,6 +318,36 @@
   </si>
   <si>
     <t>Reservar con al menos 2 horas de anticipación. Prohibido el consumo de alimentos en la sala.</t>
+  </si>
+  <si>
+    <t>Si</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Jueves 19 de septiebre de 2024 11:00:00 AM</t>
+  </si>
+  <si>
+    <t>Sábado 21 de septiembre de 2024 4:00:00 PM</t>
+  </si>
+  <si>
+    <t>Lunes 16 de septiembre de 2024 6:00:00 AM</t>
+  </si>
+  <si>
+    <t>Martes 17 de septiembre de 2024 8:00:00 AM</t>
+  </si>
+  <si>
+    <t>Jueves 19 de septiembre de 2024 7:00:00 PM</t>
+  </si>
+  <si>
+    <t>Sábado 21 de septiembre de 2024 9:00:00 PM</t>
+  </si>
+  <si>
+    <t>Lunes 16 de septiembre de 2024 7:00:00 PM</t>
+  </si>
+  <si>
+    <t>Martes 17 de septiembre de 2024 3:00:00 PM</t>
   </si>
 </sst>
 </file>
@@ -465,9 +492,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -497,9 +521,6 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -520,8 +541,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -591,6 +618,10 @@
     </sheetDataSet>
   </externalBook>
 </externalLink>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -943,7 +974,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -951,7 +982,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -968,7 +999,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AAB45A7-2401-4156-812B-1376902CA2CF}">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B7" workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
@@ -999,32 +1030,32 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="C2" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="D2" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>43</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>44</v>
       </c>
       <c r="F2" s="7"/>
       <c r="G2" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H2" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="I2" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="J2" s="7" t="s">
         <v>46</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -1035,351 +1066,351 @@
         <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>65</v>
-      </c>
       <c r="H3" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="J3" s="24" t="s">
+      <c r="J3" s="23" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="29">
+        <v>1</v>
+      </c>
+      <c r="B4" s="29" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="31">
-        <v>1</v>
-      </c>
-      <c r="B4" s="31" t="s">
+      <c r="C4" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C4" s="32" t="s">
-        <v>66</v>
-      </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="29">
+        <v>50</v>
+      </c>
+      <c r="F4" s="29">
+        <v>60</v>
+      </c>
+      <c r="G4" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E4" s="31">
-        <v>50</v>
-      </c>
-      <c r="F4" s="31">
-        <v>60</v>
-      </c>
-      <c r="G4" s="31" t="s">
-        <v>60</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="I4" s="32" t="str">
+      <c r="I4" s="30" t="str">
         <f>[1]ConjuntoResidencial!$I$4</f>
         <v>1-Forest apartamentos</v>
       </c>
-      <c r="J4" s="33" t="str">
+      <c r="J4" s="31" t="str">
         <f>_xlfn.CONCAT(B4,"-",I4)</f>
         <v>Piscina-1-Forest apartamentos</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="34">
+      <c r="A5" s="32">
         <v>2</v>
       </c>
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="C5" s="32" t="s">
-        <v>67</v>
-      </c>
-      <c r="D5" s="35" t="s">
+      <c r="E5" s="32">
+        <v>20</v>
+      </c>
+      <c r="F5" s="32">
+        <v>120</v>
+      </c>
+      <c r="G5" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="H5" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="E5" s="34">
-        <v>20</v>
-      </c>
-      <c r="F5" s="34">
-        <v>120</v>
-      </c>
-      <c r="G5" s="34" t="s">
-        <v>60</v>
-      </c>
-      <c r="H5" s="35" t="s">
-        <v>56</v>
-      </c>
-      <c r="I5" s="32" t="str">
+      <c r="I5" s="30" t="str">
         <f>[1]ConjuntoResidencial!$I$4</f>
         <v>1-Forest apartamentos</v>
       </c>
-      <c r="J5" s="33" t="str">
+      <c r="J5" s="31" t="str">
         <f>_xlfn.CONCAT(B5,"-",I5)</f>
         <v>Gimnasio-1-Forest apartamentos</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="34">
+      <c r="A6" s="32">
         <v>3</v>
       </c>
-      <c r="B6" s="34" t="s">
-        <v>57</v>
-      </c>
-      <c r="C6" s="32" t="s">
-        <v>68</v>
+      <c r="B6" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" s="30" t="s">
+        <v>67</v>
       </c>
       <c r="D6" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" s="32">
+        <v>15</v>
+      </c>
+      <c r="F6" s="32">
+        <v>1</v>
+      </c>
+      <c r="G6" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="H6" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E6" s="34">
-        <v>15</v>
-      </c>
-      <c r="F6" s="34">
-        <v>1</v>
-      </c>
-      <c r="G6" s="34" t="s">
-        <v>61</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="I6" s="32" t="str">
+      <c r="I6" s="30" t="str">
         <f>[1]ConjuntoResidencial!$I$5</f>
         <v>2-Natural</v>
       </c>
-      <c r="J6" s="33" t="str">
+      <c r="J6" s="31" t="str">
         <f>_xlfn.CONCAT(B6,"-",I6)</f>
         <v>piscinaAdultos-2-Natural</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="A7" s="34">
+      <c r="A7" s="32">
         <v>4</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="C7" s="32" t="s">
+      <c r="D7" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="D7" s="35" t="s">
+      <c r="E7" s="32">
+        <v>100</v>
+      </c>
+      <c r="F7" s="32">
+        <v>4</v>
+      </c>
+      <c r="G7" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="H7" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="E7" s="34">
-        <v>100</v>
-      </c>
-      <c r="F7" s="34">
-        <v>4</v>
-      </c>
-      <c r="G7" s="34" t="s">
-        <v>61</v>
-      </c>
-      <c r="H7" s="35" t="s">
-        <v>72</v>
-      </c>
-      <c r="I7" s="32" t="str">
+      <c r="I7" s="30" t="str">
         <f>[1]ConjuntoResidencial!I6</f>
         <v>3-Riogrande</v>
       </c>
-      <c r="J7" s="33" t="str">
+      <c r="J7" s="31" t="str">
         <f t="shared" ref="J7:J12" si="0">_xlfn.CONCAT(B7,"-",I7)</f>
         <v>Salón de Eventos-3-Riogrande</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="34">
+      <c r="A8" s="32">
         <v>5</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="C8" s="32" t="s">
+      <c r="D8" s="33" t="s">
         <v>74</v>
       </c>
-      <c r="D8" s="35" t="s">
+      <c r="E8" s="32">
+        <v>22</v>
+      </c>
+      <c r="F8" s="32">
+        <v>90</v>
+      </c>
+      <c r="G8" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="H8" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="E8" s="34">
-        <v>22</v>
-      </c>
-      <c r="F8" s="34">
-        <v>90</v>
-      </c>
-      <c r="G8" s="34" t="s">
-        <v>60</v>
-      </c>
-      <c r="H8" s="35" t="s">
-        <v>76</v>
-      </c>
-      <c r="I8" s="32" t="str">
+      <c r="I8" s="30" t="str">
         <f>[1]ConjuntoResidencial!I7</f>
         <v>4-Bolivar</v>
       </c>
-      <c r="J8" s="33" t="str">
+      <c r="J8" s="31" t="str">
         <f t="shared" si="0"/>
         <v>Cancha de Fútbol-4-Bolivar</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A9" s="34">
+      <c r="A9" s="32">
         <v>6</v>
       </c>
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="C9" s="30" t="s">
         <v>77</v>
       </c>
-      <c r="C9" s="32" t="s">
+      <c r="D9" s="33" t="s">
         <v>78</v>
       </c>
-      <c r="D9" s="35" t="s">
+      <c r="E9" s="32">
+        <v>20</v>
+      </c>
+      <c r="F9" s="32">
+        <v>45</v>
+      </c>
+      <c r="G9" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="H9" s="33" t="s">
         <v>79</v>
       </c>
-      <c r="E9" s="34">
-        <v>20</v>
-      </c>
-      <c r="F9" s="34">
-        <v>45</v>
-      </c>
-      <c r="G9" s="34" t="s">
-        <v>60</v>
-      </c>
-      <c r="H9" s="35" t="s">
-        <v>80</v>
-      </c>
-      <c r="I9" s="32" t="str">
+      <c r="I9" s="30" t="str">
         <f>[1]ConjuntoResidencial!I5</f>
         <v>2-Natural</v>
       </c>
-      <c r="J9" s="33" t="str">
+      <c r="J9" s="31" t="str">
         <f t="shared" si="0"/>
         <v>Piscina Pequeña-2-Natural</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A10" s="34">
+      <c r="A10" s="32">
         <v>7</v>
       </c>
-      <c r="B10" s="34" t="s">
+      <c r="B10" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="C10" s="30" t="s">
         <v>81</v>
       </c>
-      <c r="C10" s="32" t="s">
+      <c r="D10" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="D10" s="35" t="s">
+      <c r="E10" s="32">
+        <v>15</v>
+      </c>
+      <c r="F10" s="32">
+        <v>2</v>
+      </c>
+      <c r="G10" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="H10" s="33" t="s">
         <v>83</v>
       </c>
-      <c r="E10" s="34">
-        <v>15</v>
-      </c>
-      <c r="F10" s="34">
-        <v>2</v>
-      </c>
-      <c r="G10" s="34" t="s">
-        <v>61</v>
-      </c>
-      <c r="H10" s="35" t="s">
-        <v>84</v>
-      </c>
-      <c r="I10" s="32" t="str">
+      <c r="I10" s="30" t="str">
         <f>[1]ConjuntoResidencial!I8</f>
         <v>5-Ventus</v>
       </c>
-      <c r="J10" s="33" t="str">
+      <c r="J10" s="31" t="str">
         <f t="shared" si="0"/>
         <v>Zona BBQ-5-Ventus</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="A11" s="34">
+      <c r="A11" s="32">
         <v>8</v>
       </c>
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="C11" s="30" t="s">
         <v>85</v>
       </c>
-      <c r="C11" s="32" t="s">
+      <c r="D11" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="D11" s="35" t="s">
+      <c r="E11" s="32">
+        <v>4</v>
+      </c>
+      <c r="F11" s="32">
+        <v>60</v>
+      </c>
+      <c r="G11" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="H11" s="33" t="s">
         <v>87</v>
       </c>
-      <c r="E11" s="34">
-        <v>4</v>
-      </c>
-      <c r="F11" s="34">
-        <v>60</v>
-      </c>
-      <c r="G11" s="34" t="s">
-        <v>60</v>
-      </c>
-      <c r="H11" s="35" t="s">
-        <v>88</v>
-      </c>
-      <c r="I11" s="32" t="str">
+      <c r="I11" s="30" t="str">
         <f>[1]ConjuntoResidencial!I6</f>
         <v>3-Riogrande</v>
       </c>
-      <c r="J11" s="33" t="str">
+      <c r="J11" s="31" t="str">
         <f t="shared" si="0"/>
         <v>Cancha de Tenis-3-Riogrande</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="34">
+      <c r="A12" s="32">
         <v>9</v>
       </c>
-      <c r="B12" s="34" t="s">
+      <c r="B12" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="C12" s="30" t="s">
         <v>89</v>
       </c>
-      <c r="C12" s="32" t="s">
+      <c r="D12" s="33" t="s">
         <v>90</v>
       </c>
-      <c r="D12" s="35" t="s">
+      <c r="E12" s="32">
+        <v>10</v>
+      </c>
+      <c r="F12" s="32">
+        <v>90</v>
+      </c>
+      <c r="G12" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="H12" s="33" t="s">
         <v>91</v>
       </c>
-      <c r="E12" s="34">
-        <v>10</v>
-      </c>
-      <c r="F12" s="34">
-        <v>90</v>
-      </c>
-      <c r="G12" s="34" t="s">
-        <v>60</v>
-      </c>
-      <c r="H12" s="35" t="s">
-        <v>92</v>
-      </c>
-      <c r="I12" s="32" t="str">
+      <c r="I12" s="30" t="str">
         <f>[1]ConjuntoResidencial!I4</f>
         <v>1-Forest apartamentos</v>
       </c>
-      <c r="J12" s="33" t="str">
+      <c r="J12" s="31" t="str">
         <f t="shared" si="0"/>
         <v>Sala de Juegos-1-Forest apartamentos</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B13" s="36"/>
-      <c r="C13" s="37"/>
-      <c r="D13" s="38"/>
-      <c r="H13" s="38"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="35"/>
+      <c r="D13" s="36"/>
+      <c r="H13" s="36"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C14" s="37"/>
-      <c r="D14" s="38"/>
-      <c r="H14" s="38"/>
+      <c r="C14" s="35"/>
+      <c r="D14" s="36"/>
+      <c r="H14" s="36"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C15" s="37"/>
-      <c r="D15" s="38"/>
-      <c r="H15" s="38"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="36"/>
+      <c r="H15" s="36"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1400,7 +1431,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1410,17 +1441,17 @@
     <col min="4" max="4" width="17.33203125" customWidth="1"/>
     <col min="5" max="5" width="46.109375" customWidth="1"/>
     <col min="6" max="6" width="44.6640625" customWidth="1"/>
-    <col min="7" max="7" width="128.44140625" customWidth="1"/>
+    <col min="7" max="7" width="136.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
       <c r="F1" s="6"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -1467,7 +1498,7 @@
       <c r="A4" s="9">
         <v>1</v>
       </c>
-      <c r="B4" s="25" t="str">
+      <c r="B4" s="24" t="str">
         <f>ZonaComun!J4</f>
         <v>Piscina-1-Forest apartamentos</v>
       </c>
@@ -1475,12 +1506,12 @@
         <v>18</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="10">
+        <v>92</v>
+      </c>
+      <c r="E4" s="39">
         <v>45553.25</v>
       </c>
-      <c r="F4" s="10">
+      <c r="F4" s="39">
         <v>45553.583333333336</v>
       </c>
       <c r="G4" s="8" t="str">
@@ -1492,24 +1523,24 @@
       <c r="A5" s="9">
         <v>2</v>
       </c>
-      <c r="B5" s="25" t="str">
+      <c r="B5" s="24" t="str">
         <f>ZonaComun!J5</f>
         <v>Gimnasio-1-Forest apartamentos</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="10">
+        <v>92</v>
+      </c>
+      <c r="E5" s="39">
         <v>45553.625</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5" s="39">
         <v>45553.875</v>
       </c>
       <c r="G5" s="8" t="str">
-        <f t="shared" ref="G5:G7" si="0">C5&amp;" "&amp;TEXT(E5,"- dd  mmmm yyyy h:mm:ss AM/PM ")&amp;" hasta "&amp;TEXT(F5,"- dd  mmmm yyyy h:mm:ss AM/PM ")&amp;"-"&amp;B5</f>
+        <f t="shared" ref="G5:G11" si="0">C5&amp;" "&amp;TEXT(E5,"- dd  mmmm yyyy h:mm:ss AM/PM ")&amp;" hasta "&amp;TEXT(F5,"- dd  mmmm yyyy h:mm:ss AM/PM ")&amp;"-"&amp;B5</f>
         <v>Agenda para residentes turno Nocturno - 18  septiembre 2024 3:00:00 p. m.  hasta - 18  septiembre 2024 9:00:00 p. m. -Gimnasio-1-Forest apartamentos</v>
       </c>
     </row>
@@ -1517,20 +1548,20 @@
       <c r="A6" s="9">
         <v>3</v>
       </c>
-      <c r="B6" s="25" t="str">
+      <c r="B6" s="24" t="str">
         <f>ZonaComun!J6</f>
         <v>piscinaAdultos-2-Natural</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="10">
+        <v>92</v>
+      </c>
+      <c r="E6" s="39">
         <v>45555.416666666664</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6" s="39">
         <v>45555.541666666664</v>
       </c>
       <c r="G6" s="8" t="str">
@@ -1542,20 +1573,20 @@
       <c r="A7" s="9">
         <v>4</v>
       </c>
-      <c r="B7" s="25" t="str">
+      <c r="B7" s="24" t="str">
         <f>ZonaComun!J7</f>
         <v>Salón de Eventos-3-Riogrande</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="10">
+        <v>92</v>
+      </c>
+      <c r="E7" s="39">
         <v>45553.333333333336</v>
       </c>
-      <c r="F7" s="10">
+      <c r="F7" s="39">
         <v>45553.5</v>
       </c>
       <c r="G7" s="8" t="str">
@@ -1567,60 +1598,104 @@
       <c r="A8" s="9">
         <v>5</v>
       </c>
-      <c r="B8" s="25" t="str">
+      <c r="B8" s="24" t="str">
         <f>ZonaComun!J8</f>
         <v>Cancha de Fútbol-4-Bolivar</v>
       </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="8"/>
+      <c r="C8" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="E8" s="39" t="s">
+        <v>94</v>
+      </c>
+      <c r="F8" s="39" t="s">
+        <v>98</v>
+      </c>
+      <c r="G8" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>Agenda para residentes turno Diurno Jueves 19 de septiebre de 2024 11:00:00 AM hasta Jueves 19 de septiembre de 2024 7:00:00 PM-Cancha de Fútbol-4-Bolivar</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="9">
         <v>6</v>
       </c>
-      <c r="B9" s="25" t="str">
+      <c r="B9" s="24" t="str">
         <f>ZonaComun!J9</f>
         <v>Piscina Pequeña-2-Natural</v>
       </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="8"/>
+      <c r="C9" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="E9" s="39" t="s">
+        <v>95</v>
+      </c>
+      <c r="F9" s="39" t="s">
+        <v>99</v>
+      </c>
+      <c r="G9" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>Agenda para residentes turno Nocturno Sábado 21 de septiembre de 2024 4:00:00 PM hasta Sábado 21 de septiembre de 2024 9:00:00 PM-Piscina Pequeña-2-Natural</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="9">
         <v>7</v>
       </c>
-      <c r="B10" s="25" t="str">
+      <c r="B10" s="24" t="str">
         <f>ZonaComun!J10</f>
         <v>Zona BBQ-5-Ventus</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="8"/>
+      <c r="C10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="E10" s="39" t="s">
+        <v>96</v>
+      </c>
+      <c r="F10" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="G10" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>Agenda para residentes turno Diurno Lunes 16 de septiembre de 2024 6:00:00 AM hasta Lunes 16 de septiembre de 2024 7:00:00 PM-Zona BBQ-5-Ventus</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="9">
         <v>8</v>
       </c>
-      <c r="B11" s="25" t="str">
+      <c r="B11" s="24" t="str">
         <f>ZonaComun!J11</f>
         <v>Cancha de Tenis-3-Riogrande</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="8"/>
+      <c r="C11" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="E11" s="39" t="s">
+        <v>97</v>
+      </c>
+      <c r="F11" s="39" t="s">
+        <v>101</v>
+      </c>
+      <c r="G11" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>Agenda para residentes Martes 17 de septiembre de 2024 8:00:00 AM hasta Martes 17 de septiembre de 2024 3:00:00 PM-Cancha de Tenis-3-Riogrande</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="39"/>
+      <c r="A12" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1655,34 +1730,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
       <c r="F1" s="6"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="C2" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="D2" s="7" t="s">
         <v>25</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>26</v>
       </c>
       <c r="E2" s="7"/>
       <c r="F2" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>27</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -1690,16 +1765,16 @@
         <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>5</v>
@@ -1709,360 +1784,360 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="11">
+      <c r="A4" s="10">
         <v>1</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="11">
+        <v>0.25</v>
+      </c>
+      <c r="D4" s="11">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E4" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="12">
-        <v>0.25</v>
-      </c>
-      <c r="D4" s="12">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="F4" s="26" t="str">
+      <c r="F4" s="25" t="str">
         <f>Agenda!$G$4</f>
         <v>Agenda para residentes turno Diurno - 18  septiembre 2024 6:00:00 a. m.  hasta - 18  septiembre 2024 2:00:00 p. m. -Piscina-1-Forest apartamentos</v>
       </c>
-      <c r="G4" s="14" t="str">
-        <f t="shared" ref="G4:G21" si="0">_xlfn.CONCAT(B4,"-",F4)</f>
+      <c r="G4" s="13" t="str">
+        <f t="shared" ref="G4:G17" si="0">_xlfn.CONCAT(B4,"-",F4)</f>
         <v>Turno 1-Agenda para residentes turno Diurno - 18  septiembre 2024 6:00:00 a. m.  hasta - 18  septiembre 2024 2:00:00 p. m. -Piscina-1-Forest apartamentos</v>
       </c>
       <c r="I4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="10">
+        <v>2</v>
+      </c>
+      <c r="B5" s="10" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="11">
-        <v>2</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" s="12">
+      <c r="C5" s="11">
         <v>0.33333333333333331</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="11">
         <v>0.41666666666666669</v>
       </c>
-      <c r="E5" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="F5" s="26" t="str">
+      <c r="E5" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="25" t="str">
         <f>Agenda!$G$4</f>
         <v>Agenda para residentes turno Diurno - 18  septiembre 2024 6:00:00 a. m.  hasta - 18  septiembre 2024 2:00:00 p. m. -Piscina-1-Forest apartamentos</v>
       </c>
-      <c r="G5" s="14" t="str">
+      <c r="G5" s="13" t="str">
         <f t="shared" si="0"/>
         <v>Turno 2-Agenda para residentes turno Diurno - 18  septiembre 2024 6:00:00 a. m.  hasta - 18  septiembre 2024 2:00:00 p. m. -Piscina-1-Forest apartamentos</v>
       </c>
       <c r="I5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="11">
+      <c r="A6" s="10">
         <v>3</v>
       </c>
-      <c r="B6" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C6" s="12">
+      <c r="B6" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="11">
         <v>0.41666666666666669</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D6" s="11">
         <v>0.5</v>
       </c>
-      <c r="E6" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="F6" s="26" t="str">
+      <c r="E6" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="25" t="str">
         <f>Agenda!$G$4</f>
         <v>Agenda para residentes turno Diurno - 18  septiembre 2024 6:00:00 a. m.  hasta - 18  septiembre 2024 2:00:00 p. m. -Piscina-1-Forest apartamentos</v>
       </c>
-      <c r="G6" s="14" t="str">
+      <c r="G6" s="13" t="str">
         <f t="shared" si="0"/>
         <v>Turno 3-Agenda para residentes turno Diurno - 18  septiembre 2024 6:00:00 a. m.  hasta - 18  septiembre 2024 2:00:00 p. m. -Piscina-1-Forest apartamentos</v>
       </c>
       <c r="I6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="10">
+        <v>4</v>
+      </c>
+      <c r="B7" s="10" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="11">
-        <v>4</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="C7" s="12">
+      <c r="C7" s="11">
         <v>0.54166666666666696</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="11">
         <v>0.58333333333333404</v>
       </c>
-      <c r="E7" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="F7" s="26" t="str">
+      <c r="E7" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="25" t="str">
         <f>Agenda!$G$4</f>
         <v>Agenda para residentes turno Diurno - 18  septiembre 2024 6:00:00 a. m.  hasta - 18  septiembre 2024 2:00:00 p. m. -Piscina-1-Forest apartamentos</v>
       </c>
-      <c r="G7" s="14" t="str">
+      <c r="G7" s="13" t="str">
         <f t="shared" si="0"/>
         <v>Turno 4-Agenda para residentes turno Diurno - 18  septiembre 2024 6:00:00 a. m.  hasta - 18  septiembre 2024 2:00:00 p. m. -Piscina-1-Forest apartamentos</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="15">
+      <c r="A8" s="14">
         <v>5</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="15">
+        <v>0.625</v>
+      </c>
+      <c r="D8" s="15">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E8" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="16">
-        <v>0.625</v>
-      </c>
-      <c r="D8" s="16">
-        <v>0.70833333333333337</v>
-      </c>
-      <c r="E8" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="F8" s="27" t="str">
+      <c r="F8" s="26" t="str">
         <f>Agenda!$G$5</f>
         <v>Agenda para residentes turno Nocturno - 18  septiembre 2024 3:00:00 p. m.  hasta - 18  septiembre 2024 9:00:00 p. m. -Gimnasio-1-Forest apartamentos</v>
       </c>
-      <c r="G8" s="14" t="str">
+      <c r="G8" s="13" t="str">
         <f t="shared" si="0"/>
         <v>Turno 1-Agenda para residentes turno Nocturno - 18  septiembre 2024 3:00:00 p. m.  hasta - 18  septiembre 2024 9:00:00 p. m. -Gimnasio-1-Forest apartamentos</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="15">
+      <c r="A9" s="14">
         <v>6</v>
       </c>
-      <c r="B9" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="C9" s="16">
+      <c r="B9" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="15">
         <v>0.70833333333333337</v>
       </c>
-      <c r="D9" s="16">
+      <c r="D9" s="15">
         <v>0.79166666666666663</v>
       </c>
-      <c r="E9" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="F9" s="27" t="str">
+      <c r="E9" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" s="26" t="str">
         <f>Agenda!$G$5</f>
         <v>Agenda para residentes turno Nocturno - 18  septiembre 2024 3:00:00 p. m.  hasta - 18  septiembre 2024 9:00:00 p. m. -Gimnasio-1-Forest apartamentos</v>
       </c>
-      <c r="G9" s="14" t="str">
+      <c r="G9" s="13" t="str">
         <f t="shared" si="0"/>
         <v>Turno 2-Agenda para residentes turno Nocturno - 18  septiembre 2024 3:00:00 p. m.  hasta - 18  septiembre 2024 9:00:00 p. m. -Gimnasio-1-Forest apartamentos</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="15">
+      <c r="A10" s="14">
         <v>7</v>
       </c>
-      <c r="B10" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="C10" s="16">
+      <c r="B10" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="15">
         <v>0.79166666666666663</v>
       </c>
-      <c r="D10" s="16">
+      <c r="D10" s="15">
         <v>0.875</v>
       </c>
-      <c r="E10" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="F10" s="27" t="str">
+      <c r="E10" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" s="26" t="str">
         <f>Agenda!$G$5</f>
         <v>Agenda para residentes turno Nocturno - 18  septiembre 2024 3:00:00 p. m.  hasta - 18  septiembre 2024 9:00:00 p. m. -Gimnasio-1-Forest apartamentos</v>
       </c>
-      <c r="G10" s="14" t="str">
+      <c r="G10" s="13" t="str">
         <f t="shared" si="0"/>
         <v>Turno 3-Agenda para residentes turno Nocturno - 18  septiembre 2024 3:00:00 p. m.  hasta - 18  septiembre 2024 9:00:00 p. m. -Gimnasio-1-Forest apartamentos</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="18">
+      <c r="A11" s="17">
         <v>8</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="18">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="D11" s="18">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="E11" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="19">
-        <v>0.91666666666666663</v>
-      </c>
-      <c r="D11" s="19">
-        <v>0.95833333333333337</v>
-      </c>
-      <c r="E11" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="F11" s="28" t="str">
+      <c r="F11" s="27" t="str">
         <f>Agenda!$G$6</f>
         <v>Agenda para residentes - 20  septiembre 2024 10:00:00 a. m.  hasta - 20  septiembre 2024 1:00:00 p. m. -piscinaAdultos-2-Natural</v>
       </c>
-      <c r="G11" s="14" t="str">
+      <c r="G11" s="13" t="str">
         <f t="shared" si="0"/>
         <v>Turno 1-Agenda para residentes - 20  septiembre 2024 10:00:00 a. m.  hasta - 20  septiembre 2024 1:00:00 p. m. -piscinaAdultos-2-Natural</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="18">
+      <c r="A12" s="17">
         <v>9</v>
       </c>
-      <c r="B12" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" s="19">
+      <c r="B12" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="18">
         <v>0.45833333333333331</v>
       </c>
-      <c r="D12" s="19">
+      <c r="D12" s="18">
         <v>0.5</v>
       </c>
-      <c r="E12" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="F12" s="28" t="str">
+      <c r="E12" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12" s="27" t="str">
         <f>Agenda!$G$6</f>
         <v>Agenda para residentes - 20  septiembre 2024 10:00:00 a. m.  hasta - 20  septiembre 2024 1:00:00 p. m. -piscinaAdultos-2-Natural</v>
       </c>
-      <c r="G12" s="14" t="str">
+      <c r="G12" s="13" t="str">
         <f t="shared" si="0"/>
         <v>Turno 2-Agenda para residentes - 20  septiembre 2024 10:00:00 a. m.  hasta - 20  septiembre 2024 1:00:00 p. m. -piscinaAdultos-2-Natural</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="18">
+      <c r="A13" s="17">
         <v>10</v>
       </c>
-      <c r="B13" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="19">
+      <c r="B13" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="18">
         <v>0.5</v>
       </c>
-      <c r="D13" s="19">
+      <c r="D13" s="18">
         <v>0.54166666666666663</v>
       </c>
-      <c r="E13" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="F13" s="28" t="str">
+      <c r="E13" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" s="27" t="str">
         <f>Agenda!$G$6</f>
         <v>Agenda para residentes - 20  septiembre 2024 10:00:00 a. m.  hasta - 20  septiembre 2024 1:00:00 p. m. -piscinaAdultos-2-Natural</v>
       </c>
-      <c r="G13" s="14" t="str">
+      <c r="G13" s="13" t="str">
         <f t="shared" si="0"/>
         <v>Turno 3-Agenda para residentes - 20  septiembre 2024 10:00:00 a. m.  hasta - 20  septiembre 2024 1:00:00 p. m. -piscinaAdultos-2-Natural</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="21">
+      <c r="A14" s="20">
         <v>11</v>
       </c>
-      <c r="B14" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" s="22">
+      <c r="B14" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="21">
         <v>0.33333333333333331</v>
       </c>
-      <c r="D14" s="22">
+      <c r="D14" s="21">
         <v>0.375</v>
       </c>
-      <c r="E14" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="F14" s="29" t="str">
+      <c r="E14" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="F14" s="28" t="str">
         <f>Agenda!$G$7</f>
         <v>Agenda para dias de mantenimiento - 18  septiembre 2024 8:00:00 a. m.  hasta - 18  septiembre 2024 12:00:00 p. m. -Salón de Eventos-3-Riogrande</v>
       </c>
-      <c r="G14" s="14" t="str">
+      <c r="G14" s="13" t="str">
         <f t="shared" si="0"/>
         <v>Turno 1-Agenda para dias de mantenimiento - 18  septiembre 2024 8:00:00 a. m.  hasta - 18  septiembre 2024 12:00:00 p. m. -Salón de Eventos-3-Riogrande</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="21">
+      <c r="A15" s="20">
         <v>12</v>
       </c>
-      <c r="B15" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="C15" s="22">
+      <c r="B15" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="21">
         <v>0.375</v>
       </c>
-      <c r="D15" s="22">
+      <c r="D15" s="21">
         <v>0.41666666666666702</v>
       </c>
-      <c r="E15" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="F15" s="29" t="str">
+      <c r="E15" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="F15" s="28" t="str">
         <f>Agenda!$G$7</f>
         <v>Agenda para dias de mantenimiento - 18  septiembre 2024 8:00:00 a. m.  hasta - 18  septiembre 2024 12:00:00 p. m. -Salón de Eventos-3-Riogrande</v>
       </c>
-      <c r="G15" s="14" t="str">
+      <c r="G15" s="13" t="str">
         <f t="shared" si="0"/>
         <v>Turno 2-Agenda para dias de mantenimiento - 18  septiembre 2024 8:00:00 a. m.  hasta - 18  septiembre 2024 12:00:00 p. m. -Salón de Eventos-3-Riogrande</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="21">
+      <c r="A16" s="20">
         <v>13</v>
       </c>
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="21">
+        <v>0.41666666666666702</v>
+      </c>
+      <c r="D16" s="21">
+        <v>0.45833333333333398</v>
+      </c>
+      <c r="E16" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="22">
-        <v>0.41666666666666702</v>
-      </c>
-      <c r="D16" s="22">
-        <v>0.45833333333333398</v>
-      </c>
-      <c r="E16" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="F16" s="29" t="str">
+      <c r="F16" s="28" t="str">
         <f>Agenda!$G$7</f>
         <v>Agenda para dias de mantenimiento - 18  septiembre 2024 8:00:00 a. m.  hasta - 18  septiembre 2024 12:00:00 p. m. -Salón de Eventos-3-Riogrande</v>
       </c>
-      <c r="G16" s="14" t="str">
+      <c r="G16" s="13" t="str">
         <f>_xlfn.CONCAT(B16,"-",F16)</f>
         <v>Turno 3-Agenda para dias de mantenimiento - 18  septiembre 2024 8:00:00 a. m.  hasta - 18  septiembre 2024 12:00:00 p. m. -Salón de Eventos-3-Riogrande</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="21">
+      <c r="A17" s="20">
         <v>14</v>
       </c>
-      <c r="B17" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" s="22">
+      <c r="B17" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="21">
         <v>0.45833333333333398</v>
       </c>
-      <c r="D17" s="22">
+      <c r="D17" s="21">
         <v>0.500000000000001</v>
       </c>
-      <c r="E17" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="F17" s="29" t="str">
+      <c r="E17" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="F17" s="28" t="str">
         <f>Agenda!$G$7</f>
         <v>Agenda para dias de mantenimiento - 18  septiembre 2024 8:00:00 a. m.  hasta - 18  septiembre 2024 12:00:00 p. m. -Salón de Eventos-3-Riogrande</v>
       </c>
-      <c r="G17" s="14" t="str">
+      <c r="G17" s="13" t="str">
         <f t="shared" si="0"/>
         <v>Turno 4-Agenda para dias de mantenimiento - 18  septiembre 2024 8:00:00 a. m.  hasta - 18  septiembre 2024 12:00:00 p. m. -Salón de Eventos-3-Riogrande</v>
       </c>

</xml_diff>

<commit_message>
Poniendo bien las descripciones del muetreo de datos y modificando el nombre de los atributos con lowerCamelCase
</commit_message>
<xml_diff>
--- a/Doo-Doc/Nueva Version Victus/MuestreoDatos/Agenda Muestreo Datos.xlsx
+++ b/Doo-Doc/Nueva Version Victus/MuestreoDatos/Agenda Muestreo Datos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uconet-my.sharepoint.com/personal/juan_avendano1956_uco_net_co/Documents/Documents/victus-doc/Doo-Doc/Nueva Version Victus/MuestreoDatos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Music\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{B89AD7CE-8143-4AEB-B50A-6CDFA11B9B51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4A63616D-7A8A-4FD5-AAE1-35AFDD49DE25}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7AF4F49-760C-479F-897F-11346DC13983}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{2D4B8DA6-DD27-486A-88C5-FC69C929F1D2}"/>
+    <workbookView xWindow="2250" yWindow="3600" windowWidth="15855" windowHeight="15345" activeTab="3" xr2:uid="{2D4B8DA6-DD27-486A-88C5-FC69C929F1D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Objetos de dominio" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="98">
   <si>
     <t>Nombre</t>
   </si>
@@ -74,12 +74,6 @@
     <t>Es un dato que representa la zona común con la que está relacionada la agenda especifica.</t>
   </si>
   <si>
-    <t>Es el nombre con el que se conocera la agenda para un día especifico.</t>
-  </si>
-  <si>
-    <t>Una misma agenda no puede repetirse para una zona comun</t>
-  </si>
-  <si>
     <t>Identificador</t>
   </si>
   <si>
@@ -116,33 +110,15 @@
     <t>Es un dato que hace que cada turno sea único.</t>
   </si>
   <si>
-    <t>Este dato representa el nombre y número con el que se va a concoer el turno</t>
-  </si>
-  <si>
     <t>Es un dato que representa la hora de inicio del turno.</t>
   </si>
   <si>
     <t>Es un dato que representa la hora de finalización del turno.</t>
   </si>
   <si>
-    <t>Este dato represdenta con que agenda está relacionada el turno.</t>
-  </si>
-  <si>
     <t>Un turno especifico no puede repetirse dentro de la misma agenda</t>
   </si>
   <si>
-    <t>Número de turno</t>
-  </si>
-  <si>
-    <t>Hora inicio</t>
-  </si>
-  <si>
-    <t>Hora finalización</t>
-  </si>
-  <si>
-    <t>Estado</t>
-  </si>
-  <si>
     <t>Turno 1</t>
   </si>
   <si>
@@ -170,9 +146,6 @@
     <t>Es un dato que representa al nombre de una zona comun.</t>
   </si>
   <si>
-    <t>Es te atributo hace referencia a la imagen que va a acompañar a la zona común para mayor facilidad a la hora de identificarlo.</t>
-  </si>
-  <si>
     <t>Es un dato que representa el formato de texto de una descripción para la zona común.</t>
   </si>
   <si>
@@ -188,12 +161,6 @@
     <t>No es posible tener más de una zona común con el mismo nombre para un mismo conjunto residencial.</t>
   </si>
   <si>
-    <t>Imagen</t>
-  </si>
-  <si>
-    <t>Normas</t>
-  </si>
-  <si>
     <t>Combinación única 1</t>
   </si>
   <si>
@@ -230,18 +197,6 @@
     <t>Hora</t>
   </si>
   <si>
-    <t>Es un dato que representa cuantos minutos son permitidos por uso en un dia la zona común</t>
-  </si>
-  <si>
-    <t>Capacidad de personas</t>
-  </si>
-  <si>
-    <t>tiempo de uso</t>
-  </si>
-  <si>
-    <t>Unidad de tiempo de uso</t>
-  </si>
-  <si>
     <t>piscina001.jpg</t>
   </si>
   <si>
@@ -321,6 +276,66 @@
   </si>
   <si>
     <t>Reservar con al menos 2 horas de anticipación. Prohibido el consumo de alimentos en la sala.</t>
+  </si>
+  <si>
+    <t>Este atributo hace referencia a la imagen que va a acompañar a la zona común para mayor facilidad a la hora de identificarlo.</t>
+  </si>
+  <si>
+    <t>Este es le dato que representa el tiempo de uso por numero entero de residente</t>
+  </si>
+  <si>
+    <t>Es un dato que representa la unidad de la cual el tiempo de va a definir</t>
+  </si>
+  <si>
+    <t>Este es un dato tipo texto que representa el nombre de como se llama la agenda que se esta programando</t>
+  </si>
+  <si>
+    <t>Este dato es un tipo logico que representa si esta disponible o no la agenda</t>
+  </si>
+  <si>
+    <t>Este dato representa la fecha de hora de inicio en la cual empieza la agenda.</t>
+  </si>
+  <si>
+    <t>Este dato representa la fecha de hora final en la cual finaliza una agenda.</t>
+  </si>
+  <si>
+    <t>Una misma agenda no puede repetirse para el mismo nombre de agenda, fecha de inicio, fecha final y zona comun</t>
+  </si>
+  <si>
+    <t>Este dato representa el nombre y número con el que se va a concoer el turno por defecto la palabra "Turno" y luego un numero consecutivo</t>
+  </si>
+  <si>
+    <t>Este dato es de tipo logico el cual dice si esta disponible o no disponible un turno</t>
+  </si>
+  <si>
+    <t>Este dato representa con que agenda está relacionada el turno.</t>
+  </si>
+  <si>
+    <t>numeroDeTurno</t>
+  </si>
+  <si>
+    <t>horaInicio</t>
+  </si>
+  <si>
+    <t>horaFinalizacion</t>
+  </si>
+  <si>
+    <t>imagen</t>
+  </si>
+  <si>
+    <t>descripcion</t>
+  </si>
+  <si>
+    <t>capacidadDePersonas</t>
+  </si>
+  <si>
+    <t>tiempoDeUso</t>
+  </si>
+  <si>
+    <t>unidadDeTiempoDeUso</t>
+  </si>
+  <si>
+    <t>normas</t>
   </si>
 </sst>
 </file>
@@ -497,9 +512,6 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -520,12 +532,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -594,7 +609,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -916,13 +931,13 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.6640625" customWidth="1"/>
-    <col min="2" max="2" width="58.33203125" customWidth="1"/>
+    <col min="1" max="1" width="27.7109375" customWidth="1"/>
+    <col min="2" max="2" width="58.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -930,7 +945,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -938,20 +953,20 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -968,22 +983,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AAB45A7-2401-4156-812B-1376902CA2CF}">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="21.6640625" customWidth="1"/>
-    <col min="3" max="3" width="24.6640625" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" customWidth="1"/>
     <col min="4" max="4" width="27" customWidth="1"/>
-    <col min="5" max="7" width="21.6640625" customWidth="1"/>
+    <col min="5" max="6" width="21.7109375" customWidth="1"/>
+    <col min="7" max="7" width="23.7109375" customWidth="1"/>
     <col min="8" max="8" width="15" customWidth="1"/>
-    <col min="9" max="9" width="23.6640625" customWidth="1"/>
-    <col min="10" max="10" width="33.109375" customWidth="1"/>
+    <col min="9" max="9" width="23.7109375" customWidth="1"/>
+    <col min="10" max="10" width="35.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>7</v>
       </c>
@@ -997,399 +1014,401 @@
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>42</v>
+        <v>78</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="F2" s="7"/>
+        <v>35</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>79</v>
+      </c>
       <c r="G2" s="7" t="s">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>48</v>
+        <v>92</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>1</v>
+        <v>93</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>63</v>
+        <v>94</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>64</v>
+        <v>95</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>65</v>
+        <v>96</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>49</v>
+        <v>97</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="J3" s="24" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="30">
+        <v>1</v>
+      </c>
+      <c r="B4" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="30">
         <v>50</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="31">
-        <v>1</v>
-      </c>
-      <c r="B4" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="C4" s="32" t="s">
-        <v>66</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E4" s="31">
-        <v>50</v>
-      </c>
-      <c r="F4" s="31">
+      <c r="F4" s="30">
         <v>60</v>
       </c>
-      <c r="G4" s="31" t="s">
-        <v>60</v>
+      <c r="G4" s="30" t="s">
+        <v>49</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="I4" s="32" t="str">
+        <v>42</v>
+      </c>
+      <c r="I4" s="31" t="str">
         <f>[1]ConjuntoResidencial!$I$4</f>
         <v>1-Forest apartamentos</v>
       </c>
-      <c r="J4" s="33" t="str">
+      <c r="J4" s="32" t="str">
         <f>_xlfn.CONCAT(B4,"-",I4)</f>
         <v>Piscina-1-Forest apartamentos</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="34">
+    <row r="5" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A5" s="33">
         <v>2</v>
       </c>
-      <c r="B5" s="34" t="s">
-        <v>54</v>
-      </c>
-      <c r="C5" s="32" t="s">
-        <v>67</v>
-      </c>
-      <c r="D5" s="35" t="s">
-        <v>55</v>
-      </c>
-      <c r="E5" s="34">
+      <c r="B5" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" s="33">
         <v>20</v>
       </c>
-      <c r="F5" s="34">
+      <c r="F5" s="33">
         <v>120</v>
       </c>
-      <c r="G5" s="34" t="s">
-        <v>60</v>
-      </c>
-      <c r="H5" s="35" t="s">
-        <v>56</v>
-      </c>
-      <c r="I5" s="32" t="str">
+      <c r="G5" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="H5" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="I5" s="31" t="str">
         <f>[1]ConjuntoResidencial!$I$4</f>
         <v>1-Forest apartamentos</v>
       </c>
-      <c r="J5" s="33" t="str">
+      <c r="J5" s="32" t="str">
         <f>_xlfn.CONCAT(B5,"-",I5)</f>
         <v>Gimnasio-1-Forest apartamentos</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="34">
+    <row r="6" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A6" s="33">
         <v>3</v>
       </c>
-      <c r="B6" s="34" t="s">
-        <v>57</v>
-      </c>
-      <c r="C6" s="32" t="s">
-        <v>68</v>
+      <c r="B6" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="31" t="s">
+        <v>53</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E6" s="34">
+        <v>41</v>
+      </c>
+      <c r="E6" s="33">
         <v>15</v>
       </c>
-      <c r="F6" s="34">
+      <c r="F6" s="33">
         <v>1</v>
       </c>
-      <c r="G6" s="34" t="s">
-        <v>61</v>
+      <c r="G6" s="33" t="s">
+        <v>50</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="I6" s="32" t="str">
+        <v>42</v>
+      </c>
+      <c r="I6" s="31" t="str">
         <f>[1]ConjuntoResidencial!$I$5</f>
         <v>2-Natural</v>
       </c>
-      <c r="J6" s="33" t="str">
+      <c r="J6" s="32" t="str">
         <f>_xlfn.CONCAT(B6,"-",I6)</f>
         <v>piscinaAdultos-2-Natural</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="A7" s="34">
+    <row r="7" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+      <c r="A7" s="33">
         <v>4</v>
       </c>
-      <c r="B7" s="34" t="s">
-        <v>69</v>
-      </c>
-      <c r="C7" s="32" t="s">
-        <v>70</v>
-      </c>
-      <c r="D7" s="35" t="s">
-        <v>71</v>
-      </c>
-      <c r="E7" s="34">
+      <c r="B7" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="E7" s="33">
         <v>100</v>
       </c>
-      <c r="F7" s="34">
+      <c r="F7" s="33">
         <v>4</v>
       </c>
-      <c r="G7" s="34" t="s">
-        <v>61</v>
-      </c>
-      <c r="H7" s="35" t="s">
-        <v>72</v>
-      </c>
-      <c r="I7" s="32" t="str">
+      <c r="G7" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="H7" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="I7" s="31" t="str">
         <f>[1]ConjuntoResidencial!I6</f>
         <v>3-Riogrande</v>
       </c>
-      <c r="J7" s="33" t="str">
+      <c r="J7" s="32" t="str">
         <f t="shared" ref="J7:J12" si="0">_xlfn.CONCAT(B7,"-",I7)</f>
         <v>Salón de Eventos-3-Riogrande</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="34">
+    <row r="8" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+      <c r="A8" s="33">
         <v>5</v>
       </c>
-      <c r="B8" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="C8" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="D8" s="35" t="s">
-        <v>75</v>
-      </c>
-      <c r="E8" s="34">
+      <c r="B8" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="31" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" s="33">
         <v>22</v>
       </c>
-      <c r="F8" s="34">
+      <c r="F8" s="33">
         <v>90</v>
       </c>
-      <c r="G8" s="34" t="s">
-        <v>60</v>
-      </c>
-      <c r="H8" s="35" t="s">
-        <v>76</v>
-      </c>
-      <c r="I8" s="32" t="str">
+      <c r="G8" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="H8" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="I8" s="31" t="str">
         <f>[1]ConjuntoResidencial!I7</f>
         <v>4-Bolivar</v>
       </c>
-      <c r="J8" s="33" t="str">
+      <c r="J8" s="32" t="str">
         <f t="shared" si="0"/>
         <v>Cancha de Fútbol-4-Bolivar</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A9" s="34">
+    <row r="9" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+      <c r="A9" s="33">
         <v>6</v>
       </c>
-      <c r="B9" s="34" t="s">
-        <v>77</v>
-      </c>
-      <c r="C9" s="32" t="s">
-        <v>78</v>
-      </c>
-      <c r="D9" s="35" t="s">
-        <v>79</v>
-      </c>
-      <c r="E9" s="34">
+      <c r="B9" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="D9" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="E9" s="33">
         <v>20</v>
       </c>
-      <c r="F9" s="34">
+      <c r="F9" s="33">
         <v>45</v>
       </c>
-      <c r="G9" s="34" t="s">
-        <v>60</v>
-      </c>
-      <c r="H9" s="35" t="s">
-        <v>80</v>
-      </c>
-      <c r="I9" s="32" t="str">
+      <c r="G9" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="H9" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="I9" s="31" t="str">
         <f>[1]ConjuntoResidencial!I5</f>
         <v>2-Natural</v>
       </c>
-      <c r="J9" s="33" t="str">
+      <c r="J9" s="32" t="str">
         <f t="shared" si="0"/>
         <v>Piscina Pequeña-2-Natural</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A10" s="34">
+    <row r="10" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="A10" s="33">
         <v>7</v>
       </c>
-      <c r="B10" s="34" t="s">
-        <v>81</v>
-      </c>
-      <c r="C10" s="32" t="s">
-        <v>82</v>
-      </c>
-      <c r="D10" s="35" t="s">
-        <v>83</v>
-      </c>
-      <c r="E10" s="34">
+      <c r="B10" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="D10" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="E10" s="33">
         <v>15</v>
       </c>
-      <c r="F10" s="34">
+      <c r="F10" s="33">
         <v>2</v>
       </c>
-      <c r="G10" s="34" t="s">
-        <v>61</v>
-      </c>
-      <c r="H10" s="35" t="s">
-        <v>84</v>
-      </c>
-      <c r="I10" s="32" t="str">
+      <c r="G10" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="H10" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="I10" s="31" t="str">
         <f>[1]ConjuntoResidencial!I8</f>
         <v>5-Ventus</v>
       </c>
-      <c r="J10" s="33" t="str">
+      <c r="J10" s="32" t="str">
         <f t="shared" si="0"/>
         <v>Zona BBQ-5-Ventus</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="A11" s="34">
+    <row r="11" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="A11" s="33">
         <v>8</v>
       </c>
-      <c r="B11" s="34" t="s">
-        <v>85</v>
-      </c>
-      <c r="C11" s="32" t="s">
-        <v>86</v>
-      </c>
-      <c r="D11" s="35" t="s">
-        <v>87</v>
-      </c>
-      <c r="E11" s="34">
+      <c r="B11" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="D11" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="E11" s="33">
         <v>4</v>
       </c>
-      <c r="F11" s="34">
+      <c r="F11" s="33">
         <v>60</v>
       </c>
-      <c r="G11" s="34" t="s">
-        <v>60</v>
-      </c>
-      <c r="H11" s="35" t="s">
-        <v>88</v>
-      </c>
-      <c r="I11" s="32" t="str">
+      <c r="G11" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="H11" s="34" t="s">
+        <v>73</v>
+      </c>
+      <c r="I11" s="31" t="str">
         <f>[1]ConjuntoResidencial!I6</f>
         <v>3-Riogrande</v>
       </c>
-      <c r="J11" s="33" t="str">
+      <c r="J11" s="32" t="str">
         <f t="shared" si="0"/>
         <v>Cancha de Tenis-3-Riogrande</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="34">
+    <row r="12" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+      <c r="A12" s="33">
         <v>9</v>
       </c>
-      <c r="B12" s="34" t="s">
-        <v>89</v>
-      </c>
-      <c r="C12" s="32" t="s">
+      <c r="B12" s="33" t="s">
+        <v>74</v>
+      </c>
+      <c r="C12" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="D12" s="34" t="s">
+        <v>76</v>
+      </c>
+      <c r="E12" s="33">
+        <v>10</v>
+      </c>
+      <c r="F12" s="33">
         <v>90</v>
       </c>
-      <c r="D12" s="35" t="s">
-        <v>91</v>
-      </c>
-      <c r="E12" s="34">
-        <v>10</v>
-      </c>
-      <c r="F12" s="34">
-        <v>90</v>
-      </c>
-      <c r="G12" s="34" t="s">
-        <v>60</v>
-      </c>
-      <c r="H12" s="35" t="s">
-        <v>92</v>
-      </c>
-      <c r="I12" s="32" t="str">
+      <c r="G12" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="H12" s="34" t="s">
+        <v>77</v>
+      </c>
+      <c r="I12" s="31" t="str">
         <f>[1]ConjuntoResidencial!I4</f>
         <v>1-Forest apartamentos</v>
       </c>
-      <c r="J12" s="33" t="str">
+      <c r="J12" s="32" t="str">
         <f t="shared" si="0"/>
         <v>Sala de Juegos-1-Forest apartamentos</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B13" s="36"/>
-      <c r="C13" s="37"/>
-      <c r="D13" s="38"/>
-      <c r="H13" s="38"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C14" s="37"/>
-      <c r="D14" s="38"/>
-      <c r="H14" s="38"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C15" s="37"/>
-      <c r="D15" s="38"/>
-      <c r="H15" s="38"/>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="35"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="37"/>
+      <c r="H13" s="37"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C14" s="36"/>
+      <c r="D14" s="37"/>
+      <c r="H14" s="37"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C15" s="36"/>
+      <c r="D15" s="37"/>
+      <c r="H15" s="37"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" location="Objetos de dominio!A1" display="Objetos de dominio!A1" xr:uid="{CBEDEE6C-22FE-43B3-89F1-C741AF6805E9}"/>
-    <hyperlink ref="B1" location="Objetos de dominio!A1" display="Objetos de dominio!A1" xr:uid="{5049E57E-E139-4ADD-9C47-2609FB902FFB}"/>
-    <hyperlink ref="J1" location="Objetos de dominio!A1" display="Objetos de dominio!A1" xr:uid="{C8B3E4EF-57B4-4A4C-936C-454FCCF14785}"/>
-    <hyperlink ref="I3" location="ConjuntoResidencial!A1" display="ConjuntoResidencial" xr:uid="{FA68C03A-4D40-437E-A7E7-34175C992F59}"/>
-    <hyperlink ref="I4" location="ConjuntoResidencial!A5" display="ConjuntoResidencial!A5" xr:uid="{EB5BF42C-0DC8-4822-8A90-7F46EFD084D1}"/>
-    <hyperlink ref="I5" location="ConjuntoResidencial!A5" display="ConjuntoResidencial!A5" xr:uid="{50984DC8-E1AF-407A-A8DF-68C2FF5A2144}"/>
-    <hyperlink ref="I6" location="ConjuntoResidencial!A5" display="ConjuntoResidencial!A5" xr:uid="{BA2EDD1E-B40E-479F-88EC-DCC6DF46D04F}"/>
+    <hyperlink ref="A1" location="Objetos de dominio!A1" display="Objetos de dominio!A1" xr:uid="{86880221-D35A-4DFB-9D0F-98DE4788A220}"/>
+    <hyperlink ref="B1" location="Objetos de dominio!A1" display="Objetos de dominio!A1" xr:uid="{DBBAE10B-A1FB-42D3-9992-A55767ECF823}"/>
+    <hyperlink ref="J1" location="Objetos de dominio!A1" display="Objetos de dominio!A1" xr:uid="{072E8954-4FF6-4D79-B766-D8306B6F90DE}"/>
+    <hyperlink ref="I3" location="ConjuntoResidencial!A1" display="ConjuntoResidencial" xr:uid="{688254C5-E31B-4EE3-B9A6-0E0B69B3C8FB}"/>
+    <hyperlink ref="I4" location="ConjuntoResidencial!A5" display="ConjuntoResidencial!A5" xr:uid="{55C76EB6-6C1C-469C-97C0-0252C3A09D13}"/>
+    <hyperlink ref="I5" location="ConjuntoResidencial!A5" display="ConjuntoResidencial!A5" xr:uid="{2AC631C3-5164-43BE-AAED-B4CC64A47F9C}"/>
+    <hyperlink ref="I6" location="ConjuntoResidencial!A5" display="ConjuntoResidencial!A5" xr:uid="{05C6D3D6-646C-4A57-8331-FF8D9B28F085}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1399,71 +1418,77 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4578BD62-C112-42DC-9A20-08C85087F0AF}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="40.44140625" customWidth="1"/>
-    <col min="3" max="3" width="40.5546875" customWidth="1"/>
-    <col min="4" max="4" width="17.33203125" customWidth="1"/>
-    <col min="5" max="5" width="46.109375" customWidth="1"/>
-    <col min="6" max="6" width="44.6640625" customWidth="1"/>
-    <col min="7" max="7" width="128.44140625" customWidth="1"/>
+    <col min="2" max="2" width="40.42578125" customWidth="1"/>
+    <col min="3" max="3" width="40.5703125" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" customWidth="1"/>
+    <col min="5" max="5" width="46.140625" customWidth="1"/>
+    <col min="6" max="6" width="44.7109375" customWidth="1"/>
+    <col min="7" max="7" width="136.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="30" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
+      <c r="C2" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>82</v>
+      </c>
       <c r="E2" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="G3" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>1</v>
       </c>
@@ -1472,10 +1497,10 @@
         <v>Piscina-1-Forest apartamentos</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E4" s="10">
         <v>45553.25</v>
@@ -1488,7 +1513,7 @@
         <v>Agenda para residentes turno Diurno - 18  septiembre 2024 6:00:00 a. m.  hasta - 18  septiembre 2024 2:00:00 p. m. -Piscina-1-Forest apartamentos</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <v>2</v>
       </c>
@@ -1497,10 +1522,10 @@
         <v>Gimnasio-1-Forest apartamentos</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E5" s="10">
         <v>45553.625</v>
@@ -1513,7 +1538,7 @@
         <v>Agenda para residentes turno Nocturno - 18  septiembre 2024 3:00:00 p. m.  hasta - 18  septiembre 2024 9:00:00 p. m. -Gimnasio-1-Forest apartamentos</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>3</v>
       </c>
@@ -1522,10 +1547,10 @@
         <v>piscinaAdultos-2-Natural</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E6" s="10">
         <v>45555.416666666664</v>
@@ -1538,7 +1563,7 @@
         <v>Agenda para residentes - 20  septiembre 2024 10:00:00 a. m.  hasta - 20  septiembre 2024 1:00:00 p. m. -piscinaAdultos-2-Natural</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
         <v>4</v>
       </c>
@@ -1547,10 +1572,10 @@
         <v>Salón de Eventos-3-Riogrande</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E7" s="10">
         <v>45553.333333333336</v>
@@ -1563,7 +1588,7 @@
         <v>Agenda para dias de mantenimiento - 18  septiembre 2024 8:00:00 a. m.  hasta - 18  septiembre 2024 12:00:00 p. m. -Salón de Eventos-3-Riogrande</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>5</v>
       </c>
@@ -1577,7 +1602,7 @@
       <c r="F8" s="10"/>
       <c r="G8" s="8"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <v>6</v>
       </c>
@@ -1591,7 +1616,7 @@
       <c r="F9" s="10"/>
       <c r="G9" s="8"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>7</v>
       </c>
@@ -1605,7 +1630,7 @@
       <c r="F10" s="10"/>
       <c r="G10" s="8"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>8</v>
       </c>
@@ -1619,8 +1644,8 @@
       <c r="F11" s="10"/>
       <c r="G11" s="8"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="39"/>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1638,82 +1663,84 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1481DBD8-8614-460B-A4B3-0BC96282F835}">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.109375" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="4" width="21.6640625" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" customWidth="1"/>
-    <col min="6" max="6" width="123.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="130.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="21.7109375" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" customWidth="1"/>
+    <col min="6" max="6" width="133.7109375" customWidth="1"/>
+    <col min="7" max="7" width="140.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="30" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="E2" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7" t="s">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="11">
         <v>1</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="C4" s="12">
         <v>0.25</v>
@@ -1722,26 +1749,23 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="F4" s="26" t="str">
         <f>Agenda!$G$4</f>
         <v>Agenda para residentes turno Diurno - 18  septiembre 2024 6:00:00 a. m.  hasta - 18  septiembre 2024 2:00:00 p. m. -Piscina-1-Forest apartamentos</v>
       </c>
       <c r="G4" s="14" t="str">
-        <f t="shared" ref="G4:G21" si="0">_xlfn.CONCAT(B4,"-",F4)</f>
+        <f t="shared" ref="G4:G17" si="0">_xlfn.CONCAT(B4,"-",F4)</f>
         <v>Turno 1-Agenda para residentes turno Diurno - 18  septiembre 2024 6:00:00 a. m.  hasta - 18  septiembre 2024 2:00:00 p. m. -Piscina-1-Forest apartamentos</v>
       </c>
-      <c r="I4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="11">
         <v>2</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C5" s="12">
         <v>0.33333333333333331</v>
@@ -1750,7 +1774,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="F5" s="26" t="str">
         <f>Agenda!$G$4</f>
@@ -1760,16 +1784,13 @@
         <f t="shared" si="0"/>
         <v>Turno 2-Agenda para residentes turno Diurno - 18  septiembre 2024 6:00:00 a. m.  hasta - 18  septiembre 2024 2:00:00 p. m. -Piscina-1-Forest apartamentos</v>
       </c>
-      <c r="I5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="11">
         <v>3</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C6" s="12">
         <v>0.41666666666666669</v>
@@ -1778,7 +1799,7 @@
         <v>0.5</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="F6" s="26" t="str">
         <f>Agenda!$G$4</f>
@@ -1788,16 +1809,13 @@
         <f t="shared" si="0"/>
         <v>Turno 3-Agenda para residentes turno Diurno - 18  septiembre 2024 6:00:00 a. m.  hasta - 18  septiembre 2024 2:00:00 p. m. -Piscina-1-Forest apartamentos</v>
       </c>
-      <c r="I6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="11">
         <v>4</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C7" s="12">
         <v>0.54166666666666696</v>
@@ -1806,7 +1824,7 @@
         <v>0.58333333333333404</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="F7" s="26" t="str">
         <f>Agenda!$G$4</f>
@@ -1817,12 +1835,12 @@
         <v>Turno 4-Agenda para residentes turno Diurno - 18  septiembre 2024 6:00:00 a. m.  hasta - 18  septiembre 2024 2:00:00 p. m. -Piscina-1-Forest apartamentos</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="15">
         <v>5</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="C8" s="16">
         <v>0.625</v>
@@ -1831,7 +1849,7 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="F8" s="27" t="str">
         <f>Agenda!$G$5</f>
@@ -1842,12 +1860,12 @@
         <v>Turno 1-Agenda para residentes turno Nocturno - 18  septiembre 2024 3:00:00 p. m.  hasta - 18  septiembre 2024 9:00:00 p. m. -Gimnasio-1-Forest apartamentos</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="15">
         <v>6</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C9" s="16">
         <v>0.70833333333333337</v>
@@ -1856,7 +1874,7 @@
         <v>0.79166666666666663</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="F9" s="27" t="str">
         <f>Agenda!$G$5</f>
@@ -1867,12 +1885,12 @@
         <v>Turno 2-Agenda para residentes turno Nocturno - 18  septiembre 2024 3:00:00 p. m.  hasta - 18  septiembre 2024 9:00:00 p. m. -Gimnasio-1-Forest apartamentos</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="15">
         <v>7</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C10" s="16">
         <v>0.79166666666666663</v>
@@ -1881,7 +1899,7 @@
         <v>0.875</v>
       </c>
       <c r="E10" s="17" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="F10" s="27" t="str">
         <f>Agenda!$G$5</f>
@@ -1892,12 +1910,12 @@
         <v>Turno 3-Agenda para residentes turno Nocturno - 18  septiembre 2024 3:00:00 p. m.  hasta - 18  septiembre 2024 9:00:00 p. m. -Gimnasio-1-Forest apartamentos</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="18">
         <v>8</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="C11" s="19">
         <v>0.91666666666666663</v>
@@ -1906,7 +1924,7 @@
         <v>0.95833333333333337</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="F11" s="28" t="str">
         <f>Agenda!$G$6</f>
@@ -1917,12 +1935,12 @@
         <v>Turno 1-Agenda para residentes - 20  septiembre 2024 10:00:00 a. m.  hasta - 20  septiembre 2024 1:00:00 p. m. -piscinaAdultos-2-Natural</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="18">
         <v>9</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C12" s="19">
         <v>0.45833333333333331</v>
@@ -1931,7 +1949,7 @@
         <v>0.5</v>
       </c>
       <c r="E12" s="20" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="F12" s="28" t="str">
         <f>Agenda!$G$6</f>
@@ -1942,12 +1960,12 @@
         <v>Turno 2-Agenda para residentes - 20  septiembre 2024 10:00:00 a. m.  hasta - 20  septiembre 2024 1:00:00 p. m. -piscinaAdultos-2-Natural</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="18">
         <v>10</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C13" s="19">
         <v>0.5</v>
@@ -1956,7 +1974,7 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="E13" s="20" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="F13" s="28" t="str">
         <f>Agenda!$G$6</f>
@@ -1967,12 +1985,12 @@
         <v>Turno 3-Agenda para residentes - 20  septiembre 2024 10:00:00 a. m.  hasta - 20  septiembre 2024 1:00:00 p. m. -piscinaAdultos-2-Natural</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="21">
         <v>11</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="C14" s="22">
         <v>0.33333333333333331</v>
@@ -1981,7 +1999,7 @@
         <v>0.375</v>
       </c>
       <c r="E14" s="23" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="F14" s="29" t="str">
         <f>Agenda!$G$7</f>
@@ -1992,12 +2010,12 @@
         <v>Turno 1-Agenda para dias de mantenimiento - 18  septiembre 2024 8:00:00 a. m.  hasta - 18  septiembre 2024 12:00:00 p. m. -Salón de Eventos-3-Riogrande</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="21">
         <v>12</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C15" s="22">
         <v>0.375</v>
@@ -2006,7 +2024,7 @@
         <v>0.41666666666666702</v>
       </c>
       <c r="E15" s="23" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="F15" s="29" t="str">
         <f>Agenda!$G$7</f>
@@ -2017,12 +2035,12 @@
         <v>Turno 2-Agenda para dias de mantenimiento - 18  septiembre 2024 8:00:00 a. m.  hasta - 18  septiembre 2024 12:00:00 p. m. -Salón de Eventos-3-Riogrande</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="21">
         <v>13</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C16" s="22">
         <v>0.41666666666666702</v>
@@ -2031,7 +2049,7 @@
         <v>0.45833333333333398</v>
       </c>
       <c r="E16" s="23" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="F16" s="29" t="str">
         <f>Agenda!$G$7</f>
@@ -2042,12 +2060,12 @@
         <v>Turno 3-Agenda para dias de mantenimiento - 18  septiembre 2024 8:00:00 a. m.  hasta - 18  septiembre 2024 12:00:00 p. m. -Salón de Eventos-3-Riogrande</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="21">
         <v>14</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C17" s="22">
         <v>0.45833333333333398</v>
@@ -2056,7 +2074,7 @@
         <v>0.500000000000001</v>
       </c>
       <c r="E17" s="23" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="F17" s="29" t="str">
         <f>Agenda!$G$7</f>

</xml_diff>

<commit_message>
Modificacion y organización de muestreo
</commit_message>
<xml_diff>
--- a/Doo-Doc/Nueva Version Victus/MuestreoDatos/Agenda Muestreo Datos.xlsx
+++ b/Doo-Doc/Nueva Version Victus/MuestreoDatos/Agenda Muestreo Datos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Music\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josez\Documents\Universidad IngeSistemas\Diseño Orientado a Objetos(DOO)\VictusProyect\victus-doc\Doo-Doc\Nueva Version Victus\MuestreoDatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7AF4F49-760C-479F-897F-11346DC13983}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F45A935-4C6A-4612-A209-83A851451F8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2250" yWindow="3600" windowWidth="15855" windowHeight="15345" activeTab="3" xr2:uid="{2D4B8DA6-DD27-486A-88C5-FC69C929F1D2}"/>
+    <workbookView minimized="1" xWindow="2916" yWindow="3708" windowWidth="17280" windowHeight="8880" activeTab="3" xr2:uid="{2D4B8DA6-DD27-486A-88C5-FC69C929F1D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Objetos de dominio" sheetId="1" r:id="rId1"/>
@@ -931,13 +931,13 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" customWidth="1"/>
-    <col min="2" max="2" width="58.28515625" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" customWidth="1"/>
+    <col min="2" max="2" width="58.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -945,7 +945,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -953,7 +953,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -961,7 +961,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -987,20 +987,20 @@
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" customWidth="1"/>
-    <col min="2" max="2" width="21.7109375" customWidth="1"/>
-    <col min="3" max="3" width="24.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" customWidth="1"/>
+    <col min="3" max="3" width="24.6640625" customWidth="1"/>
     <col min="4" max="4" width="27" customWidth="1"/>
-    <col min="5" max="6" width="21.7109375" customWidth="1"/>
-    <col min="7" max="7" width="23.7109375" customWidth="1"/>
+    <col min="5" max="6" width="21.6640625" customWidth="1"/>
+    <col min="7" max="7" width="23.6640625" customWidth="1"/>
     <col min="8" max="8" width="15" customWidth="1"/>
-    <col min="9" max="9" width="23.7109375" customWidth="1"/>
-    <col min="10" max="10" width="35.42578125" customWidth="1"/>
+    <col min="9" max="9" width="23.6640625" customWidth="1"/>
+    <col min="10" max="10" width="35.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>7</v>
       </c>
@@ -1014,7 +1014,7 @@
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>32</v>
       </c>
@@ -1046,7 +1046,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -1078,7 +1078,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="30">
         <v>1</v>
       </c>
@@ -1112,7 +1112,7 @@
         <v>Piscina-1-Forest apartamentos</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" s="33">
         <v>2</v>
       </c>
@@ -1146,7 +1146,7 @@
         <v>Gimnasio-1-Forest apartamentos</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="33">
         <v>3</v>
       </c>
@@ -1180,7 +1180,7 @@
         <v>piscinaAdultos-2-Natural</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A7" s="33">
         <v>4</v>
       </c>
@@ -1214,7 +1214,7 @@
         <v>Salón de Eventos-3-Riogrande</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A8" s="33">
         <v>5</v>
       </c>
@@ -1248,7 +1248,7 @@
         <v>Cancha de Fútbol-4-Bolivar</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A9" s="33">
         <v>6</v>
       </c>
@@ -1282,7 +1282,7 @@
         <v>Piscina Pequeña-2-Natural</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A10" s="33">
         <v>7</v>
       </c>
@@ -1316,7 +1316,7 @@
         <v>Zona BBQ-5-Ventus</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A11" s="33">
         <v>8</v>
       </c>
@@ -1350,7 +1350,7 @@
         <v>Cancha de Tenis-3-Riogrande</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A12" s="33">
         <v>9</v>
       </c>
@@ -1384,18 +1384,18 @@
         <v>Sala de Juegos-1-Forest apartamentos</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B13" s="35"/>
       <c r="C13" s="36"/>
       <c r="D13" s="37"/>
       <c r="H13" s="37"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C14" s="36"/>
       <c r="D14" s="37"/>
       <c r="H14" s="37"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C15" s="36"/>
       <c r="D15" s="37"/>
       <c r="H15" s="37"/>
@@ -1422,17 +1422,17 @@
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="40.42578125" customWidth="1"/>
-    <col min="3" max="3" width="40.5703125" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" customWidth="1"/>
-    <col min="5" max="5" width="46.140625" customWidth="1"/>
-    <col min="6" max="6" width="44.7109375" customWidth="1"/>
-    <col min="7" max="7" width="136.5703125" customWidth="1"/>
+    <col min="2" max="2" width="40.44140625" customWidth="1"/>
+    <col min="3" max="3" width="40.5546875" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" customWidth="1"/>
+    <col min="5" max="5" width="46.109375" customWidth="1"/>
+    <col min="6" max="6" width="44.6640625" customWidth="1"/>
+    <col min="7" max="7" width="136.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="39" t="s">
         <v>7</v>
       </c>
@@ -1442,7 +1442,7 @@
       <c r="E1" s="39"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>8</v>
       </c>
@@ -1465,7 +1465,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -1488,7 +1488,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="9">
         <v>1</v>
       </c>
@@ -1513,7 +1513,7 @@
         <v>Agenda para residentes turno Diurno - 18  septiembre 2024 6:00:00 a. m.  hasta - 18  septiembre 2024 2:00:00 p. m. -Piscina-1-Forest apartamentos</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="9">
         <v>2</v>
       </c>
@@ -1538,7 +1538,7 @@
         <v>Agenda para residentes turno Nocturno - 18  septiembre 2024 3:00:00 p. m.  hasta - 18  septiembre 2024 9:00:00 p. m. -Gimnasio-1-Forest apartamentos</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="9">
         <v>3</v>
       </c>
@@ -1563,7 +1563,7 @@
         <v>Agenda para residentes - 20  septiembre 2024 10:00:00 a. m.  hasta - 20  septiembre 2024 1:00:00 p. m. -piscinaAdultos-2-Natural</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="9">
         <v>4</v>
       </c>
@@ -1588,7 +1588,7 @@
         <v>Agenda para dias de mantenimiento - 18  septiembre 2024 8:00:00 a. m.  hasta - 18  septiembre 2024 12:00:00 p. m. -Salón de Eventos-3-Riogrande</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="9">
         <v>5</v>
       </c>
@@ -1602,7 +1602,7 @@
       <c r="F8" s="10"/>
       <c r="G8" s="8"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="9">
         <v>6</v>
       </c>
@@ -1616,7 +1616,7 @@
       <c r="F9" s="10"/>
       <c r="G9" s="8"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="9">
         <v>7</v>
       </c>
@@ -1630,7 +1630,7 @@
       <c r="F10" s="10"/>
       <c r="G10" s="8"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="9">
         <v>8</v>
       </c>
@@ -1644,7 +1644,7 @@
       <c r="F11" s="10"/>
       <c r="G11" s="8"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="38"/>
     </row>
   </sheetData>
@@ -1669,17 +1669,17 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="1" max="1" width="14.109375" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="4" width="21.7109375" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" customWidth="1"/>
-    <col min="6" max="6" width="133.7109375" customWidth="1"/>
-    <col min="7" max="7" width="140.7109375" customWidth="1"/>
+    <col min="3" max="4" width="21.6640625" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" customWidth="1"/>
+    <col min="6" max="6" width="133.6640625" customWidth="1"/>
+    <col min="7" max="7" width="140.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="39" t="s">
         <v>7</v>
       </c>
@@ -1689,7 +1689,7 @@
       <c r="E1" s="39"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>21</v>
       </c>
@@ -1712,7 +1712,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -1735,7 +1735,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="11">
         <v>1</v>
       </c>
@@ -1760,7 +1760,7 @@
         <v>Turno 1-Agenda para residentes turno Diurno - 18  septiembre 2024 6:00:00 a. m.  hasta - 18  septiembre 2024 2:00:00 p. m. -Piscina-1-Forest apartamentos</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="11">
         <v>2</v>
       </c>
@@ -1785,7 +1785,7 @@
         <v>Turno 2-Agenda para residentes turno Diurno - 18  septiembre 2024 6:00:00 a. m.  hasta - 18  septiembre 2024 2:00:00 p. m. -Piscina-1-Forest apartamentos</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="11">
         <v>3</v>
       </c>
@@ -1810,7 +1810,7 @@
         <v>Turno 3-Agenda para residentes turno Diurno - 18  septiembre 2024 6:00:00 a. m.  hasta - 18  septiembre 2024 2:00:00 p. m. -Piscina-1-Forest apartamentos</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="11">
         <v>4</v>
       </c>
@@ -1835,7 +1835,7 @@
         <v>Turno 4-Agenda para residentes turno Diurno - 18  septiembre 2024 6:00:00 a. m.  hasta - 18  septiembre 2024 2:00:00 p. m. -Piscina-1-Forest apartamentos</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="15">
         <v>5</v>
       </c>
@@ -1860,7 +1860,7 @@
         <v>Turno 1-Agenda para residentes turno Nocturno - 18  septiembre 2024 3:00:00 p. m.  hasta - 18  septiembre 2024 9:00:00 p. m. -Gimnasio-1-Forest apartamentos</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="15">
         <v>6</v>
       </c>
@@ -1885,7 +1885,7 @@
         <v>Turno 2-Agenda para residentes turno Nocturno - 18  septiembre 2024 3:00:00 p. m.  hasta - 18  septiembre 2024 9:00:00 p. m. -Gimnasio-1-Forest apartamentos</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="15">
         <v>7</v>
       </c>
@@ -1910,7 +1910,7 @@
         <v>Turno 3-Agenda para residentes turno Nocturno - 18  septiembre 2024 3:00:00 p. m.  hasta - 18  septiembre 2024 9:00:00 p. m. -Gimnasio-1-Forest apartamentos</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="18">
         <v>8</v>
       </c>
@@ -1935,7 +1935,7 @@
         <v>Turno 1-Agenda para residentes - 20  septiembre 2024 10:00:00 a. m.  hasta - 20  septiembre 2024 1:00:00 p. m. -piscinaAdultos-2-Natural</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="18">
         <v>9</v>
       </c>
@@ -1960,7 +1960,7 @@
         <v>Turno 2-Agenda para residentes - 20  septiembre 2024 10:00:00 a. m.  hasta - 20  septiembre 2024 1:00:00 p. m. -piscinaAdultos-2-Natural</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="18">
         <v>10</v>
       </c>
@@ -1985,7 +1985,7 @@
         <v>Turno 3-Agenda para residentes - 20  septiembre 2024 10:00:00 a. m.  hasta - 20  septiembre 2024 1:00:00 p. m. -piscinaAdultos-2-Natural</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="21">
         <v>11</v>
       </c>
@@ -2010,7 +2010,7 @@
         <v>Turno 1-Agenda para dias de mantenimiento - 18  septiembre 2024 8:00:00 a. m.  hasta - 18  septiembre 2024 12:00:00 p. m. -Salón de Eventos-3-Riogrande</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="21">
         <v>12</v>
       </c>
@@ -2035,7 +2035,7 @@
         <v>Turno 2-Agenda para dias de mantenimiento - 18  septiembre 2024 8:00:00 a. m.  hasta - 18  septiembre 2024 12:00:00 p. m. -Salón de Eventos-3-Riogrande</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="21">
         <v>13</v>
       </c>
@@ -2060,7 +2060,7 @@
         <v>Turno 3-Agenda para dias de mantenimiento - 18  septiembre 2024 8:00:00 a. m.  hasta - 18  septiembre 2024 12:00:00 p. m. -Salón de Eventos-3-Riogrande</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="21">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
finalizando event Storming de COnjuntos residenciales, Residentes y Agendas
</commit_message>
<xml_diff>
--- a/Doo-Doc/Nueva Version Victus/MuestreoDatos/Agenda Muestreo Datos.xlsx
+++ b/Doo-Doc/Nueva Version Victus/MuestreoDatos/Agenda Muestreo Datos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\DOO 2024 BD\DOO\victus-doc\Doo-Doc\Nueva Version Victus\MuestreoDatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A08565F6-CFFA-45DE-84D2-3A4FD06D18EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1C1BFA9-9677-42BB-A2B3-276620FEC457}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="3900" windowWidth="28800" windowHeight="15285" activeTab="3" xr2:uid="{2D4B8DA6-DD27-486A-88C5-FC69C929F1D2}"/>
+    <workbookView xWindow="16695" yWindow="4440" windowWidth="16800" windowHeight="14190" activeTab="3" xr2:uid="{2D4B8DA6-DD27-486A-88C5-FC69C929F1D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Objetos de dominio" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="108">
   <si>
     <t>Nombre</t>
   </si>
@@ -356,9 +356,6 @@
     <t>NoDisponible</t>
   </si>
   <si>
-    <t>No es posible tener un nombre con la misma agenda para la misma hora de inicio y hora final del turno para una misma turno.</t>
-  </si>
-  <si>
     <t>Objeto de dominio que representa a cada una de las zonas comúnes que tendrán una agenda y respectivos turnos.</t>
   </si>
   <si>
@@ -366,6 +363,9 @@
   </si>
   <si>
     <t>Objeto de dominio que representa uno de los turnos que representan un bloque de tiempo que el residente podrá reservar.</t>
+  </si>
+  <si>
+    <t>No es posible tener un nombre con la misma agenda para la misma hora de inicio y hora final  para una misma turno.</t>
   </si>
 </sst>
 </file>
@@ -1123,7 +1123,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -1131,7 +1131,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -1139,7 +1139,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -1590,8 +1590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4578BD62-C112-42DC-9A20-08C85087F0AF}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView topLeftCell="F1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1937,10 +1937,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1481DBD8-8614-460B-A4B3-0BC96282F835}">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1983,7 +1983,7 @@
         <v>76</v>
       </c>
       <c r="G2" s="34" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -2540,11 +2540,6 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F30" s="62"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F31" t="s">
-        <v>98</v>
-      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>